<commit_message>
updated balde and producao - base 07/01/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-01.xlsx
+++ b/first-atlas/producao_2026-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A87243-DFC3-4F0A-9C4E-10182E1D9B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2301E5D-0FB3-4341-9596-69170EDAFFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
+    <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="332">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -345,6 +345,693 @@
   </si>
   <si>
     <t>THAIS CRISTINA RESENDE SOUZA</t>
+  </si>
+  <si>
+    <t>Ainda nao iniciou a abertura de conta</t>
+  </si>
+  <si>
+    <t>12619968000180</t>
+  </si>
+  <si>
+    <t>MERCOSUL MATERIAIS DE CONSTRUCAO LTDA</t>
+  </si>
+  <si>
+    <t>Ricardo Cirino Mendes Caetano</t>
+  </si>
+  <si>
+    <t>INDICAÇÃO</t>
+  </si>
+  <si>
+    <t>45492401000144</t>
+  </si>
+  <si>
+    <t>D V CANDIDO ENXOVAIS LTDA</t>
+  </si>
+  <si>
+    <t>11888134000107</t>
+  </si>
+  <si>
+    <t>PW SERVICOS DE COBRANCA LTDA</t>
+  </si>
+  <si>
+    <t>PENDÊNCIA DOC</t>
+  </si>
+  <si>
+    <t>47457427000187</t>
+  </si>
+  <si>
+    <t>DENIS SALVATORE SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>64247704000146</t>
+  </si>
+  <si>
+    <t>ROCKS ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>11388233000120</t>
+  </si>
+  <si>
+    <t>INISOL MANUTENCAO INDUSTRIAL LTDA</t>
+  </si>
+  <si>
+    <t>Gabriela Dias Lima Fria</t>
+  </si>
+  <si>
+    <t>28865733000108</t>
+  </si>
+  <si>
+    <t>IVAN MACHADO LOBO LTDA</t>
+  </si>
+  <si>
+    <t>Giovana Vitoria da Silva</t>
+  </si>
+  <si>
+    <t>47624037000154</t>
+  </si>
+  <si>
+    <t>ECOSOL SOLUCOES AMBIENTAIS LTDA</t>
+  </si>
+  <si>
+    <t>36954685000152</t>
+  </si>
+  <si>
+    <t>ROGER ANDRE ALVES DE MOURA</t>
+  </si>
+  <si>
+    <t>18015346000129</t>
+  </si>
+  <si>
+    <t>NILSON FERNANDES DE MACEDO</t>
+  </si>
+  <si>
+    <t>20384264000101</t>
+  </si>
+  <si>
+    <t>NOSSA MARCA COSMETICOS LTDA</t>
+  </si>
+  <si>
+    <t>50435540000176</t>
+  </si>
+  <si>
+    <t>PETROVIX ASFALTOS LTDA</t>
+  </si>
+  <si>
+    <t>31770296000153</t>
+  </si>
+  <si>
+    <t>MOACIR MALASPINA</t>
+  </si>
+  <si>
+    <t>49783270000105</t>
+  </si>
+  <si>
+    <t>D M AURA ZELADORIA PATRIMONIAL LTDA</t>
+  </si>
+  <si>
+    <t>Mariana Gabriela Ferreira Barboza</t>
+  </si>
+  <si>
+    <t>62324396000180</t>
+  </si>
+  <si>
+    <t>THIAGO BATISTA GUEDES LTDA</t>
+  </si>
+  <si>
+    <t>Maria Luisa Ribeiro da Silva</t>
+  </si>
+  <si>
+    <t>48364587000144</t>
+  </si>
+  <si>
+    <t>JURA MAX MARTELINHO DE OURO LTDA</t>
+  </si>
+  <si>
+    <t>05819980000172</t>
+  </si>
+  <si>
+    <t>JOAO RAFAEL ESCUDEIRO INFORMATICA</t>
+  </si>
+  <si>
+    <t>09647194000196</t>
+  </si>
+  <si>
+    <t>FABIANO PEDRAZZI</t>
+  </si>
+  <si>
+    <t>34112133000171</t>
+  </si>
+  <si>
+    <t>DANIELE DA SILVA MACHADO SANT ANA 08520576796</t>
+  </si>
+  <si>
+    <t>42785818000107</t>
+  </si>
+  <si>
+    <t>53670082000148</t>
+  </si>
+  <si>
+    <t>STUDIO 3 TURISMO &amp; EVENTOS LTDA</t>
+  </si>
+  <si>
+    <t>23656040000191</t>
+  </si>
+  <si>
+    <t>JK IMOVEIS E ASSESSORIA LTDA</t>
+  </si>
+  <si>
+    <t>22115790000193</t>
+  </si>
+  <si>
+    <t>TENNESSE TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>29037333000177</t>
+  </si>
+  <si>
+    <t>FELIPE SILVA DA COSTA</t>
+  </si>
+  <si>
+    <t>64218120000142</t>
+  </si>
+  <si>
+    <t>D G DE PAULA IMOBILIARIA</t>
+  </si>
+  <si>
+    <t>Stephany Eduarda Pereira</t>
+  </si>
+  <si>
+    <t>44173067000101</t>
+  </si>
+  <si>
+    <t>LENITA PRADO ROUPAS E ACESSORIOS LTDA</t>
+  </si>
+  <si>
+    <t>45142439000197</t>
+  </si>
+  <si>
+    <t>CRISTIANO SILVA VILAS BOAS SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>17487754000110</t>
+  </si>
+  <si>
+    <t>JR EXTRACAO MINERAL</t>
+  </si>
+  <si>
+    <t>64270972000189</t>
+  </si>
+  <si>
+    <t>ENG CIVIL JOAO PAULO BORGES RODRIGUES LTDA</t>
+  </si>
+  <si>
+    <t>49498867000108</t>
+  </si>
+  <si>
+    <t>ANTONIO SOARES DA SILVA JUNIOR AUTOMACAO INDUSTRIAL</t>
+  </si>
+  <si>
+    <t>53532643000142</t>
+  </si>
+  <si>
+    <t>LEONIDAS PASSOS DA SILVA</t>
+  </si>
+  <si>
+    <t>56700708000100</t>
+  </si>
+  <si>
+    <t>D' MARCELO SUPERMERCADO LTDA</t>
+  </si>
+  <si>
+    <t>20539396000157</t>
+  </si>
+  <si>
+    <t>FLEXOMAGIA REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>27298297000170</t>
+  </si>
+  <si>
+    <t>EDGAR APARECIDO TEIXEIRA FILHO</t>
+  </si>
+  <si>
+    <t>44865924000126</t>
+  </si>
+  <si>
+    <t>DROGARIA LACERDA LTDA</t>
+  </si>
+  <si>
+    <t>32618296000103</t>
+  </si>
+  <si>
+    <t>32.618.296 EDILSON FERREIRA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>31230802000111</t>
+  </si>
+  <si>
+    <t>A F M DA SILVA SERVICOS</t>
+  </si>
+  <si>
+    <t>40180074000171</t>
+  </si>
+  <si>
+    <t>CAROLINA BRAGA MOURA SERVS LTDA</t>
+  </si>
+  <si>
+    <t>35595914000127</t>
+  </si>
+  <si>
+    <t>CALEIDO COMERCIAL IMPORTADORA E EXPORTADORA LTDA</t>
+  </si>
+  <si>
+    <t>30162182000168</t>
+  </si>
+  <si>
+    <t>OFICIAL COMERCIO E SERVICO LTDA</t>
+  </si>
+  <si>
+    <t>43945733000101</t>
+  </si>
+  <si>
+    <t>ALSOROVALE SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>47228405000145</t>
+  </si>
+  <si>
+    <t>FRM MULTIMARCAS LTDA</t>
+  </si>
+  <si>
+    <t>33742866000127</t>
+  </si>
+  <si>
+    <t>AUGUSTO CESAR PINTO DE CARVALHO</t>
+  </si>
+  <si>
+    <t>74169897000118</t>
+  </si>
+  <si>
+    <t>GERTEC ENGENHARIA E SOLUCOES INDUSTRIAIS LTDA</t>
+  </si>
+  <si>
+    <t>04490423000198</t>
+  </si>
+  <si>
+    <t>SAUDE &amp; ESTETICA CINTIA PAIM BATISTA LTDA</t>
+  </si>
+  <si>
+    <t>50835184000188</t>
+  </si>
+  <si>
+    <t>JMM TRANSPORTES E DISTRIBUICAO LTDA</t>
+  </si>
+  <si>
+    <t>07572152000108</t>
+  </si>
+  <si>
+    <t>LAIRATUR LOCACAO, FRETAMENTO E TURISMO LTDA</t>
+  </si>
+  <si>
+    <t>46985770000131</t>
+  </si>
+  <si>
+    <t>GLADIUS COMBAT CENTRO DE TREINAMENTO ESPECIALIZADO LTDA</t>
+  </si>
+  <si>
+    <t>08093253000169</t>
+  </si>
+  <si>
+    <t>CENTRO AUTOMOTIVO E. R. LTDA</t>
+  </si>
+  <si>
+    <t>21375147000136</t>
+  </si>
+  <si>
+    <t>C FRANCIMAR VIEIRA FEITOSA LTDA</t>
+  </si>
+  <si>
+    <t>63847361000198</t>
+  </si>
+  <si>
+    <t>KOMBINIERTE REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>49413179000106</t>
+  </si>
+  <si>
+    <t>LAURA FERREIRA DE CAMPOS</t>
+  </si>
+  <si>
+    <t>Jhonatan Vinicius de Paula Alonso</t>
+  </si>
+  <si>
+    <t>21827303000152</t>
+  </si>
+  <si>
+    <t>JPS AUTOMOCAO LTDA</t>
+  </si>
+  <si>
+    <t>22899236000144</t>
+  </si>
+  <si>
+    <t>FERNANDO RIBEIRO DOS SANTOS LTDA</t>
+  </si>
+  <si>
+    <t>CARIMBADA</t>
+  </si>
+  <si>
+    <t>26141109000132</t>
+  </si>
+  <si>
+    <t>40270893000100</t>
+  </si>
+  <si>
+    <t>CLINICA ASSISTENCIAL FORTALECER LTDA</t>
+  </si>
+  <si>
+    <t>58709096000141</t>
+  </si>
+  <si>
+    <t>A R DA SILVA ANDAIMES LTDA</t>
+  </si>
+  <si>
+    <t>10997554000169</t>
+  </si>
+  <si>
+    <t>CONSTRUTORA ANDRADE ROCHA EMPREENDIMENTOS INCORPORACAO IMOBILIARIA LTDA</t>
+  </si>
+  <si>
+    <t>21272666000179</t>
+  </si>
+  <si>
+    <t>R L S MELLO TRANSPORTES</t>
+  </si>
+  <si>
+    <t>55600604000160</t>
+  </si>
+  <si>
+    <t>CMMC EMPREENDIMENTOS IMOBILIARIOS LTDA</t>
+  </si>
+  <si>
+    <t>11487206000104</t>
+  </si>
+  <si>
+    <t>MONTE CRISTO SERVICOS DE ALVENARIA LTDA</t>
+  </si>
+  <si>
+    <t>12319753000143</t>
+  </si>
+  <si>
+    <t>SURFDOOR REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>53172088000195</t>
+  </si>
+  <si>
+    <t>BIROSKA BAR E RESTAURANTE RIO DAS OSTRAS LTDA</t>
+  </si>
+  <si>
+    <t>03143114000189</t>
+  </si>
+  <si>
+    <t>D. L. PROPAGANDA E EVENTOS LTDA.</t>
+  </si>
+  <si>
+    <t>14003567000126</t>
+  </si>
+  <si>
+    <t>LOJAS MIL CALCADOS E CONFECCOES LTDA</t>
+  </si>
+  <si>
+    <t>17056426000160</t>
+  </si>
+  <si>
+    <t>RAIMUNDO VIEIRA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>Thayssa Gasparoto Trabuco</t>
+  </si>
+  <si>
+    <t>27076508000120</t>
+  </si>
+  <si>
+    <t>27.076.508 JONATHAN DE MAIO DOS SANTOS</t>
+  </si>
+  <si>
+    <t>39346296000132</t>
+  </si>
+  <si>
+    <t>FLAVIA LOUZADA COSENDEY GOMES</t>
+  </si>
+  <si>
+    <t>63932643000193</t>
+  </si>
+  <si>
+    <t>SUBFLEX TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>50214674000167</t>
+  </si>
+  <si>
+    <t>RB MULTIMARCAS LTDA</t>
+  </si>
+  <si>
+    <t>33007314000175</t>
+  </si>
+  <si>
+    <t>EDSON CLAIR MACHADO SANTOS</t>
+  </si>
+  <si>
+    <t>40011733000146</t>
+  </si>
+  <si>
+    <t>SW EMPREITEIRA LTDA</t>
+  </si>
+  <si>
+    <t>20160334000130</t>
+  </si>
+  <si>
+    <t>D.P. TRABALHOS EM ALTURA LTDA</t>
+  </si>
+  <si>
+    <t>20427818000100</t>
+  </si>
+  <si>
+    <t>ANDREA GOMES DE CARVALHO</t>
+  </si>
+  <si>
+    <t>35861653000140</t>
+  </si>
+  <si>
+    <t>CLEMILTON FERREIRA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>63935870000172</t>
+  </si>
+  <si>
+    <t>CIRILO MR LTDA</t>
+  </si>
+  <si>
+    <t>37793901000198</t>
+  </si>
+  <si>
+    <t>SP MERCANTIL LTDA</t>
+  </si>
+  <si>
+    <t>64017238000102</t>
+  </si>
+  <si>
+    <t>LED PERFORMANCE SERVICOS AUTOMOTIVOS LTDA</t>
+  </si>
+  <si>
+    <t>63911043000149</t>
+  </si>
+  <si>
+    <t>SOUZA &amp; RIBEIRO TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>42815362000180</t>
+  </si>
+  <si>
+    <t>W A CAR OFICINA DE REPARACAO AUTOMOTIVA LTDA</t>
+  </si>
+  <si>
+    <t>64037511000160</t>
+  </si>
+  <si>
+    <t>MATEUS DE ARAUJO ALBUQUERQUE LTDA</t>
+  </si>
+  <si>
+    <t>64012635000191</t>
+  </si>
+  <si>
+    <t>MERCEARIA DO FERA LTDA</t>
+  </si>
+  <si>
+    <t>64020180000156</t>
+  </si>
+  <si>
+    <t>CARLOS JUNIOR SOLUCAO DE GESSO E DRYWALL LTDA</t>
+  </si>
+  <si>
+    <t>39815239000155</t>
+  </si>
+  <si>
+    <t>MIX MATERIAS DE CONSTRUCAO E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>64026114000193</t>
+  </si>
+  <si>
+    <t>EXTINPORTO COMBATE INCENDIO LTDA</t>
+  </si>
+  <si>
+    <t>13013290000150</t>
+  </si>
+  <si>
+    <t>DAMARIS DESENTUPIDORA LTDA</t>
+  </si>
+  <si>
+    <t>53175168000102</t>
+  </si>
+  <si>
+    <t>ANA EGLE GONCALVES LTDA</t>
+  </si>
+  <si>
+    <t>19117917000107</t>
+  </si>
+  <si>
+    <t>FURGOES CUIABA LTDA</t>
+  </si>
+  <si>
+    <t>44828030000166</t>
+  </si>
+  <si>
+    <t>ELIANE FERNANDES ESTETICA AVANCADA E ODONTOLOGIA LTDA</t>
+  </si>
+  <si>
+    <t>61893620000191</t>
+  </si>
+  <si>
+    <t>M S ENXOVAIS LTDA</t>
+  </si>
+  <si>
+    <t>63897708000107</t>
+  </si>
+  <si>
+    <t>AP MARTINS VENDAS LTDA</t>
+  </si>
+  <si>
+    <t>32103056000168</t>
+  </si>
+  <si>
+    <t>NATANAEL FERREIRA DA SILVA</t>
+  </si>
+  <si>
+    <t>45091636000124</t>
+  </si>
+  <si>
+    <t>LINDAY ATELIER DE CALCADOS LTDA</t>
+  </si>
+  <si>
+    <t>27109367000102</t>
+  </si>
+  <si>
+    <t>CRISTIANA PEREIRA MACEDO</t>
+  </si>
+  <si>
+    <t>35900717000174</t>
+  </si>
+  <si>
+    <t>35.900.717 LEANDRO DE ARAUJO SA</t>
+  </si>
+  <si>
+    <t>64005837000106</t>
+  </si>
+  <si>
+    <t>NAHRA IMPORTS LTDA</t>
+  </si>
+  <si>
+    <t>38207614000111</t>
+  </si>
+  <si>
+    <t>FABIO ALEXANDRE FELIZARDO TRANSPORTES</t>
+  </si>
+  <si>
+    <t>63963538000111</t>
+  </si>
+  <si>
+    <t>ASAFE DECOR TRES CORACOES LTDA</t>
+  </si>
+  <si>
+    <t>55238995000115</t>
+  </si>
+  <si>
+    <t>ROSA MARIA SOUZA MOTA LTDA</t>
+  </si>
+  <si>
+    <t>10574893000132</t>
+  </si>
+  <si>
+    <t>ONFLY INTERNET LTDA</t>
+  </si>
+  <si>
+    <t>49595213000100</t>
+  </si>
+  <si>
+    <t>TATI RAQUEL PIRES LTDA</t>
+  </si>
+  <si>
+    <t>62247207000112</t>
+  </si>
+  <si>
+    <t>CINTIA PEREIRA MACHADO LTDA</t>
+  </si>
+  <si>
+    <t>36908102000157</t>
+  </si>
+  <si>
+    <t>OLIVEIRA PECAS E SERVICOS AUTOMOTIVOS LTDA</t>
+  </si>
+  <si>
+    <t>30493626000148</t>
+  </si>
+  <si>
+    <t>30.493.626 MARIA GORETH DA SILVA</t>
+  </si>
+  <si>
+    <t>08640986000176</t>
+  </si>
+  <si>
+    <t>ALEX NICHIMURA PIRES</t>
+  </si>
+  <si>
+    <t>36143135000153</t>
+  </si>
+  <si>
+    <t>MIOTTI MANUTENCOES SOLUCOES EM MANUTENCAO DE MAQUINAS PARA A CONSTRUCAO CIVIL LTDA</t>
+  </si>
+  <si>
+    <t>34173154000105</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLEBER MONTEIRO DA COSTA</t>
+  </si>
+  <si>
+    <t>26926377000160</t>
+  </si>
+  <si>
+    <t>CRISTIANE DE OLIVEIRA MIEZA</t>
+  </si>
+  <si>
+    <t>23606211000178</t>
+  </si>
+  <si>
+    <t>LEMV EMPREENDIMENTOS IMOBILIARIOS LTDA</t>
+  </si>
+  <si>
+    <t>Procuracao com poderes de abrir e movimentar conta corrente junto a instituicoes financeiras com mandato vigente e devidamente assinada&lt;br&gt;&lt;br&gt;Contrato Social atualizado e registrado no orgao competente</t>
   </si>
 </sst>
 </file>
@@ -718,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A45A88-3D17-4433-986A-11075963C36F}">
   <dimension ref="A1:G1330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +1546,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1135,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1158,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1181,7 +1868,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1227,7 +1914,7 @@
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1250,7 +1937,7 @@
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1551,6 +2238,9 @@
       <c r="F36" t="s">
         <v>9</v>
       </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -1571,6 +2261,9 @@
       <c r="F37" t="s">
         <v>9</v>
       </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -1591,371 +2284,2554 @@
       <c r="F38" t="s">
         <v>9</v>
       </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+      <c r="A39" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" t="s">
+        <v>112</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" t="s">
+        <v>130</v>
+      </c>
+      <c r="D49" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B52" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B54" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" t="s">
+        <v>142</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B55" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" t="s">
+        <v>144</v>
+      </c>
+      <c r="D55" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B56" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" t="s">
+        <v>146</v>
+      </c>
+      <c r="D56" t="s">
+        <v>140</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B57" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" t="s">
+        <v>137</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B58" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B59" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" t="s">
+        <v>119</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B60" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" t="s">
+        <v>153</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B61" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" t="s">
+        <v>155</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B62" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" t="s">
+        <v>140</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B63" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" t="s">
+        <v>159</v>
+      </c>
+      <c r="D63" t="s">
+        <v>160</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B64" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" t="s">
+        <v>162</v>
+      </c>
+      <c r="D64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B65" t="s">
+        <v>163</v>
+      </c>
+      <c r="C65" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="s">
+        <v>103</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B66" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" t="s">
+        <v>166</v>
+      </c>
+      <c r="D66" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" t="s">
+        <v>103</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B67" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" t="s">
+        <v>168</v>
+      </c>
+      <c r="D67" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B68" t="s">
+        <v>169</v>
+      </c>
+      <c r="C68" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B69" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" t="s">
+        <v>172</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B70" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" t="s">
+        <v>174</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B71" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" t="s">
+        <v>176</v>
+      </c>
+      <c r="D71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B72" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" t="s">
+        <v>178</v>
+      </c>
+      <c r="D72" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B73" t="s">
+        <v>179</v>
+      </c>
+      <c r="C73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B74" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" t="s">
+        <v>137</v>
+      </c>
+      <c r="E74" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B75" t="s">
+        <v>183</v>
+      </c>
+      <c r="C75" t="s">
+        <v>184</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B76" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" t="s">
+        <v>137</v>
+      </c>
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B77" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" t="s">
+        <v>188</v>
+      </c>
+      <c r="D77" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" t="s">
+        <v>9</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B78" t="s">
+        <v>189</v>
+      </c>
+      <c r="C78" t="s">
+        <v>190</v>
+      </c>
+      <c r="D78" t="s">
+        <v>26</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B79" t="s">
+        <v>191</v>
+      </c>
+      <c r="C79" t="s">
+        <v>192</v>
+      </c>
+      <c r="D79" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B80" t="s">
+        <v>193</v>
+      </c>
+      <c r="C80" t="s">
+        <v>194</v>
+      </c>
+      <c r="D80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B81" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B82" t="s">
+        <v>197</v>
+      </c>
+      <c r="C82" t="s">
+        <v>198</v>
+      </c>
+      <c r="D82" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B83" t="s">
+        <v>199</v>
+      </c>
+      <c r="C83" t="s">
+        <v>200</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B84" t="s">
+        <v>201</v>
+      </c>
+      <c r="C84" t="s">
+        <v>202</v>
+      </c>
+      <c r="D84" t="s">
+        <v>119</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B85" t="s">
+        <v>203</v>
+      </c>
+      <c r="C85" t="s">
+        <v>204</v>
+      </c>
+      <c r="D85" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B86" t="s">
+        <v>205</v>
+      </c>
+      <c r="C86" t="s">
+        <v>206</v>
+      </c>
+      <c r="D86" t="s">
+        <v>137</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" t="s">
+        <v>112</v>
+      </c>
+      <c r="G86" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B87" t="s">
+        <v>207</v>
+      </c>
+      <c r="C87" t="s">
+        <v>208</v>
+      </c>
+      <c r="D87" t="s">
+        <v>18</v>
+      </c>
+      <c r="E87" t="s">
+        <v>15</v>
+      </c>
+      <c r="F87" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B88" t="s">
+        <v>209</v>
+      </c>
+      <c r="C88" t="s">
+        <v>210</v>
+      </c>
+      <c r="D88" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B89" t="s">
+        <v>211</v>
+      </c>
+      <c r="C89" t="s">
+        <v>212</v>
+      </c>
+      <c r="D89" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" t="s">
+        <v>15</v>
+      </c>
+      <c r="F89" t="s">
+        <v>9</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B90" t="s">
+        <v>213</v>
+      </c>
+      <c r="C90" t="s">
+        <v>214</v>
+      </c>
+      <c r="D90" t="s">
+        <v>215</v>
+      </c>
+      <c r="E90" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" t="s">
+        <v>103</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B91" t="s">
+        <v>216</v>
+      </c>
+      <c r="C91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D91" t="s">
+        <v>48</v>
+      </c>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" t="s">
+        <v>219</v>
+      </c>
+      <c r="D92" t="s">
+        <v>215</v>
+      </c>
+      <c r="E92" t="s">
+        <v>10</v>
+      </c>
+      <c r="F92" t="s">
+        <v>220</v>
+      </c>
+      <c r="G92" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B93" t="s">
+        <v>221</v>
+      </c>
+      <c r="C93" t="s">
+        <v>221</v>
+      </c>
+      <c r="D93" t="s">
+        <v>27</v>
+      </c>
+      <c r="E93" t="s">
+        <v>24</v>
+      </c>
+      <c r="F93" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B94" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" t="s">
+        <v>223</v>
+      </c>
+      <c r="D94" t="s">
+        <v>26</v>
+      </c>
+      <c r="E94" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B95" t="s">
+        <v>224</v>
+      </c>
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" t="s">
+        <v>140</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B96" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" t="s">
+        <v>227</v>
+      </c>
+      <c r="D96" t="s">
+        <v>160</v>
+      </c>
+      <c r="E96" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B97" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" t="s">
+        <v>229</v>
+      </c>
+      <c r="D97" t="s">
+        <v>16</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B98" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" t="s">
+        <v>231</v>
+      </c>
+      <c r="D98" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B99" t="s">
+        <v>232</v>
+      </c>
+      <c r="C99" t="s">
+        <v>233</v>
+      </c>
+      <c r="D99" t="s">
+        <v>16</v>
+      </c>
+      <c r="E99" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B100" t="s">
+        <v>234</v>
+      </c>
+      <c r="C100" t="s">
+        <v>235</v>
+      </c>
+      <c r="D100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C101" t="s">
+        <v>237</v>
+      </c>
+      <c r="D101" t="s">
+        <v>20</v>
+      </c>
+      <c r="E101" t="s">
+        <v>10</v>
+      </c>
+      <c r="F101" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B102" t="s">
+        <v>238</v>
+      </c>
+      <c r="C102" t="s">
+        <v>239</v>
+      </c>
+      <c r="D102" t="s">
+        <v>26</v>
+      </c>
+      <c r="E102" t="s">
+        <v>10</v>
+      </c>
+      <c r="F102" t="s">
+        <v>9</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B103" t="s">
+        <v>240</v>
+      </c>
+      <c r="C103" t="s">
+        <v>241</v>
+      </c>
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" t="s">
+        <v>10</v>
+      </c>
+      <c r="F103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B104" t="s">
+        <v>242</v>
+      </c>
+      <c r="C104" t="s">
+        <v>243</v>
+      </c>
+      <c r="D104" t="s">
+        <v>244</v>
+      </c>
+      <c r="E104" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B105" t="s">
+        <v>245</v>
+      </c>
+      <c r="C105" t="s">
+        <v>246</v>
+      </c>
+      <c r="D105" t="s">
+        <v>19</v>
+      </c>
+      <c r="E105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B106" t="s">
+        <v>247</v>
+      </c>
+      <c r="C106" t="s">
+        <v>248</v>
+      </c>
+      <c r="D106" t="s">
+        <v>27</v>
+      </c>
+      <c r="E106" t="s">
+        <v>24</v>
+      </c>
+      <c r="F106" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B107" t="s">
+        <v>249</v>
+      </c>
+      <c r="C107" t="s">
+        <v>250</v>
+      </c>
+      <c r="D107" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" t="s">
+        <v>9</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B108" t="s">
+        <v>251</v>
+      </c>
+      <c r="C108" t="s">
+        <v>252</v>
+      </c>
+      <c r="D108" t="s">
+        <v>20</v>
+      </c>
+      <c r="E108" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108" t="s">
+        <v>9</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B109" t="s">
+        <v>253</v>
+      </c>
+      <c r="C109" t="s">
+        <v>254</v>
+      </c>
+      <c r="D109" t="s">
+        <v>48</v>
+      </c>
+      <c r="E109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B110" t="s">
+        <v>255</v>
+      </c>
+      <c r="C110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D110" t="s">
+        <v>16</v>
+      </c>
+      <c r="E110" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B111" t="s">
+        <v>257</v>
+      </c>
+      <c r="C111" t="s">
+        <v>258</v>
+      </c>
+      <c r="D111" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111" t="s">
+        <v>103</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B112" t="s">
+        <v>259</v>
+      </c>
+      <c r="C112" t="s">
+        <v>260</v>
+      </c>
+      <c r="D112" t="s">
+        <v>160</v>
+      </c>
+      <c r="E112" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" t="s">
+        <v>9</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B113" t="s">
+        <v>261</v>
+      </c>
+      <c r="C113" t="s">
+        <v>262</v>
+      </c>
+      <c r="D113" t="s">
+        <v>16</v>
+      </c>
+      <c r="E113" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B114" t="s">
+        <v>263</v>
+      </c>
+      <c r="C114" t="s">
+        <v>264</v>
+      </c>
+      <c r="D114" t="s">
+        <v>16</v>
+      </c>
+      <c r="E114" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114" t="s">
+        <v>13</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B115" t="s">
+        <v>265</v>
+      </c>
+      <c r="C115" t="s">
+        <v>266</v>
+      </c>
+      <c r="D115" t="s">
+        <v>140</v>
+      </c>
+      <c r="E115" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" t="s">
+        <v>13</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B116" t="s">
+        <v>267</v>
+      </c>
+      <c r="C116" t="s">
+        <v>268</v>
+      </c>
+      <c r="D116" t="s">
+        <v>14</v>
+      </c>
+      <c r="E116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F116" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B117" t="s">
+        <v>269</v>
+      </c>
+      <c r="C117" t="s">
+        <v>270</v>
+      </c>
+      <c r="D117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B118" t="s">
+        <v>271</v>
+      </c>
+      <c r="C118" t="s">
+        <v>272</v>
+      </c>
+      <c r="D118" t="s">
+        <v>122</v>
+      </c>
+      <c r="E118" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118" t="s">
+        <v>9</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B119" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" t="s">
+        <v>274</v>
+      </c>
+      <c r="D119" t="s">
+        <v>140</v>
+      </c>
+      <c r="E119" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119" t="s">
+        <v>9</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B120" t="s">
+        <v>275</v>
+      </c>
+      <c r="C120" t="s">
+        <v>276</v>
+      </c>
+      <c r="D120" t="s">
+        <v>16</v>
+      </c>
+      <c r="E120" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120" t="s">
+        <v>9</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B121" t="s">
+        <v>277</v>
+      </c>
+      <c r="C121" t="s">
+        <v>278</v>
+      </c>
+      <c r="D121" t="s">
+        <v>7</v>
+      </c>
+      <c r="E121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" t="s">
+        <v>9</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B122" t="s">
+        <v>279</v>
+      </c>
+      <c r="C122" t="s">
+        <v>280</v>
+      </c>
+      <c r="D122" t="s">
+        <v>140</v>
+      </c>
+      <c r="E122" t="s">
+        <v>10</v>
+      </c>
+      <c r="F122" t="s">
+        <v>9</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B123" t="s">
+        <v>281</v>
+      </c>
+      <c r="C123" t="s">
+        <v>282</v>
+      </c>
+      <c r="D123" t="s">
+        <v>20</v>
+      </c>
+      <c r="E123" t="s">
+        <v>10</v>
+      </c>
+      <c r="F123" t="s">
+        <v>13</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B124" t="s">
+        <v>283</v>
+      </c>
+      <c r="C124" t="s">
+        <v>284</v>
+      </c>
+      <c r="D124" t="s">
+        <v>19</v>
+      </c>
+      <c r="E124" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124" t="s">
+        <v>9</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B125" t="s">
+        <v>285</v>
+      </c>
+      <c r="C125" t="s">
+        <v>286</v>
+      </c>
+      <c r="D125" t="s">
+        <v>11</v>
+      </c>
+      <c r="E125" t="s">
+        <v>10</v>
+      </c>
+      <c r="F125" t="s">
+        <v>13</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B126" t="s">
+        <v>287</v>
+      </c>
+      <c r="C126" t="s">
+        <v>288</v>
+      </c>
+      <c r="D126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E126" t="s">
+        <v>15</v>
+      </c>
+      <c r="F126" t="s">
+        <v>9</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B127" t="s">
+        <v>289</v>
+      </c>
+      <c r="C127" t="s">
+        <v>290</v>
+      </c>
+      <c r="D127" t="s">
+        <v>48</v>
+      </c>
+      <c r="E127" t="s">
+        <v>10</v>
+      </c>
+      <c r="F127" t="s">
+        <v>9</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B128" t="s">
+        <v>291</v>
+      </c>
+      <c r="C128" t="s">
+        <v>292</v>
+      </c>
+      <c r="D128" t="s">
+        <v>140</v>
+      </c>
+      <c r="E128" t="s">
+        <v>10</v>
+      </c>
+      <c r="F128" t="s">
+        <v>9</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B129" t="s">
+        <v>293</v>
+      </c>
+      <c r="C129" t="s">
+        <v>294</v>
+      </c>
+      <c r="D129" t="s">
+        <v>48</v>
+      </c>
+      <c r="E129" t="s">
+        <v>10</v>
+      </c>
+      <c r="F129" t="s">
+        <v>25</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B130" t="s">
+        <v>295</v>
+      </c>
+      <c r="C130" t="s">
+        <v>296</v>
+      </c>
+      <c r="D130" t="s">
+        <v>16</v>
+      </c>
+      <c r="E130" t="s">
+        <v>10</v>
+      </c>
+      <c r="F130" t="s">
+        <v>9</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B131" t="s">
+        <v>297</v>
+      </c>
+      <c r="C131" t="s">
+        <v>298</v>
+      </c>
+      <c r="D131" t="s">
+        <v>160</v>
+      </c>
+      <c r="E131" t="s">
+        <v>15</v>
+      </c>
+      <c r="F131" t="s">
+        <v>9</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B132" t="s">
+        <v>299</v>
+      </c>
+      <c r="C132" t="s">
+        <v>300</v>
+      </c>
+      <c r="D132" t="s">
+        <v>14</v>
+      </c>
+      <c r="E132" t="s">
+        <v>10</v>
+      </c>
+      <c r="F132" t="s">
+        <v>9</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B133" t="s">
+        <v>301</v>
+      </c>
+      <c r="C133" t="s">
+        <v>302</v>
+      </c>
+      <c r="D133" t="s">
+        <v>244</v>
+      </c>
+      <c r="E133" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133" t="s">
+        <v>9</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B134" t="s">
+        <v>303</v>
+      </c>
+      <c r="C134" t="s">
+        <v>304</v>
+      </c>
+      <c r="D134" t="s">
+        <v>19</v>
+      </c>
+      <c r="E134" t="s">
+        <v>10</v>
+      </c>
+      <c r="F134" t="s">
+        <v>9</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B135" t="s">
+        <v>305</v>
+      </c>
+      <c r="C135" t="s">
+        <v>306</v>
+      </c>
+      <c r="D135" t="s">
+        <v>244</v>
+      </c>
+      <c r="E135" t="s">
+        <v>8</v>
+      </c>
+      <c r="F135" t="s">
+        <v>9</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B136" t="s">
+        <v>307</v>
+      </c>
+      <c r="C136" t="s">
+        <v>308</v>
+      </c>
+      <c r="D136" t="s">
+        <v>16</v>
+      </c>
+      <c r="E136" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136" t="s">
+        <v>9</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B137" t="s">
+        <v>309</v>
+      </c>
+      <c r="C137" t="s">
+        <v>310</v>
+      </c>
+      <c r="D137" t="s">
+        <v>122</v>
+      </c>
+      <c r="E137" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" t="s">
+        <v>9</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B138" t="s">
+        <v>311</v>
+      </c>
+      <c r="C138" t="s">
+        <v>312</v>
+      </c>
+      <c r="D138" t="s">
+        <v>11</v>
+      </c>
+      <c r="E138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F138" t="s">
+        <v>9</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B139" t="s">
+        <v>313</v>
+      </c>
+      <c r="C139" t="s">
+        <v>314</v>
+      </c>
+      <c r="D139" t="s">
+        <v>20</v>
+      </c>
+      <c r="E139" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" t="s">
+        <v>9</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B140" t="s">
+        <v>315</v>
+      </c>
+      <c r="C140" t="s">
+        <v>316</v>
+      </c>
+      <c r="D140" t="s">
+        <v>19</v>
+      </c>
+      <c r="E140" t="s">
+        <v>10</v>
+      </c>
+      <c r="F140" t="s">
+        <v>9</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B141" t="s">
+        <v>317</v>
+      </c>
+      <c r="C141" t="s">
+        <v>318</v>
+      </c>
+      <c r="D141" t="s">
+        <v>14</v>
+      </c>
+      <c r="E141" t="s">
+        <v>10</v>
+      </c>
+      <c r="F141" t="s">
+        <v>9</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>46028</v>
+      </c>
+      <c r="B142" t="s">
+        <v>319</v>
+      </c>
+      <c r="C142" t="s">
+        <v>320</v>
+      </c>
+      <c r="D142" t="s">
+        <v>140</v>
+      </c>
+      <c r="E142" t="s">
+        <v>10</v>
+      </c>
+      <c r="F142" t="s">
+        <v>9</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>46029</v>
+      </c>
+      <c r="B143" t="s">
+        <v>321</v>
+      </c>
+      <c r="C143" t="s">
+        <v>322</v>
+      </c>
+      <c r="D143" t="s">
+        <v>14</v>
+      </c>
+      <c r="E143" t="s">
+        <v>10</v>
+      </c>
+      <c r="F143" t="s">
+        <v>9</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>46029</v>
+      </c>
+      <c r="B144" t="s">
+        <v>323</v>
+      </c>
+      <c r="C144" t="s">
+        <v>324</v>
+      </c>
+      <c r="D144" t="s">
+        <v>48</v>
+      </c>
+      <c r="E144" t="s">
+        <v>10</v>
+      </c>
+      <c r="F144" t="s">
+        <v>9</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>46029</v>
+      </c>
+      <c r="B145" t="s">
+        <v>325</v>
+      </c>
+      <c r="C145" t="s">
+        <v>326</v>
+      </c>
+      <c r="D145" t="s">
+        <v>140</v>
+      </c>
+      <c r="E145" t="s">
+        <v>10</v>
+      </c>
+      <c r="F145" t="s">
+        <v>9</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>46029</v>
+      </c>
+      <c r="B146" t="s">
+        <v>327</v>
+      </c>
+      <c r="C146" t="s">
+        <v>328</v>
+      </c>
+      <c r="D146" t="s">
+        <v>18</v>
+      </c>
+      <c r="E146" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" t="s">
+        <v>9</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>46029</v>
+      </c>
+      <c r="B147" t="s">
+        <v>329</v>
+      </c>
+      <c r="C147" t="s">
+        <v>330</v>
+      </c>
+      <c r="D147" t="s">
+        <v>20</v>
+      </c>
+      <c r="E147" t="s">
+        <v>10</v>
+      </c>
+      <c r="F147" t="s">
+        <v>9</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated balde and producao - base 09/01/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-01.xlsx
+++ b/first-atlas/producao_2026-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C07760-3A04-436E-9C2F-7C91773195BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655EBD8E-82A2-47DC-A224-4AFD7C8CDE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="776">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -1767,6 +1767,603 @@
   </si>
   <si>
     <t>ANÁLISE</t>
+  </si>
+  <si>
+    <t>12226807000126</t>
+  </si>
+  <si>
+    <t>ANDRESA SILVESTRINI DE SOUZA ANDRESA SILVESTRINI DE SOUZA</t>
+  </si>
+  <si>
+    <t>63499179000193</t>
+  </si>
+  <si>
+    <t>NEVILTON JUNIOR MARQUES ANDRADE</t>
+  </si>
+  <si>
+    <t>25066791000183</t>
+  </si>
+  <si>
+    <t>DOUGLAS LIXACOES LTDA</t>
+  </si>
+  <si>
+    <t>25169890000190</t>
+  </si>
+  <si>
+    <t>PAULO ROBERTO DA SILVA</t>
+  </si>
+  <si>
+    <t>09399384000131</t>
+  </si>
+  <si>
+    <t>L &amp; E SOCORRO PARACATU LTDA</t>
+  </si>
+  <si>
+    <t>64302044000159</t>
+  </si>
+  <si>
+    <t>J DE A FREITAS</t>
+  </si>
+  <si>
+    <t>15445426000126</t>
+  </si>
+  <si>
+    <t>LUCIDETE DA SILVA GOMES FERREIRA</t>
+  </si>
+  <si>
+    <t>37438292000159</t>
+  </si>
+  <si>
+    <t>ANA PRISCILA DE SOUZA DA SILVEIRA</t>
+  </si>
+  <si>
+    <t>34239826000120</t>
+  </si>
+  <si>
+    <t>ANA PAULA DE LIMA</t>
+  </si>
+  <si>
+    <t>16991514000196</t>
+  </si>
+  <si>
+    <t>ADRIANA LEITE DE OLIVEIRA CARMO</t>
+  </si>
+  <si>
+    <t>61881309000122</t>
+  </si>
+  <si>
+    <t>J.P. TORRES CONSTRUCAO LTDA</t>
+  </si>
+  <si>
+    <t>62583152000111</t>
+  </si>
+  <si>
+    <t>A MOREIRA RODRIGUES MONTAGEM LTDA</t>
+  </si>
+  <si>
+    <t>39302742000107</t>
+  </si>
+  <si>
+    <t>DANIELE GOMES DE JESUS</t>
+  </si>
+  <si>
+    <t>14279358000290</t>
+  </si>
+  <si>
+    <t>E M F DA SILVA DISTRIBUIDORA PECAS E ACESSORIOS AUTOMOTIVOS LTDA</t>
+  </si>
+  <si>
+    <t>31274906000128</t>
+  </si>
+  <si>
+    <t>JOSE S. DOS SANTOS FILHO VESTUARIO</t>
+  </si>
+  <si>
+    <t>61382643000131</t>
+  </si>
+  <si>
+    <t>ANAPOLINO FREIRE DOS SANTOS</t>
+  </si>
+  <si>
+    <t>INVÁLIDA</t>
+  </si>
+  <si>
+    <t>28558431000197</t>
+  </si>
+  <si>
+    <t>EDVAN JOSE PEREIRA</t>
+  </si>
+  <si>
+    <t>57748885000129</t>
+  </si>
+  <si>
+    <t>PEDRO MARCOS RAMOS COSTA TITO DA CRUZ SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>26431286000153</t>
+  </si>
+  <si>
+    <t>LUIZ EDUARDO BOSCHEIRO</t>
+  </si>
+  <si>
+    <t>61909386000143</t>
+  </si>
+  <si>
+    <t>MKM SERVICOS DE APOIO ADMINISTRATIVO LTDA</t>
+  </si>
+  <si>
+    <t>29909259000131</t>
+  </si>
+  <si>
+    <t>RENATO XAVIER BARCELOS</t>
+  </si>
+  <si>
+    <t>15016263000166</t>
+  </si>
+  <si>
+    <t>CLAUDIA COELHO ALBERTASSI D NADAI</t>
+  </si>
+  <si>
+    <t>27865639000196</t>
+  </si>
+  <si>
+    <t>DESCARMAX DISTRIBUIDORA LTDA</t>
+  </si>
+  <si>
+    <t>19261250000103</t>
+  </si>
+  <si>
+    <t>ELIFAS ANDRE REZENDE JARDIM</t>
+  </si>
+  <si>
+    <t>19019525000105</t>
+  </si>
+  <si>
+    <t>NILVAM GABRIEL GONCALVES</t>
+  </si>
+  <si>
+    <t>64302941000162</t>
+  </si>
+  <si>
+    <t>ATTIVA BRINDES E PERSONALIZACAO LTDA</t>
+  </si>
+  <si>
+    <t>10573013000103</t>
+  </si>
+  <si>
+    <t>DISCON COMERCIAL LTDA</t>
+  </si>
+  <si>
+    <t>08489998000141</t>
+  </si>
+  <si>
+    <t>R. M. DA CRUZ LOPES INFORMATICA</t>
+  </si>
+  <si>
+    <t>36882891000102</t>
+  </si>
+  <si>
+    <t>JOSE ANTONIO SOARES</t>
+  </si>
+  <si>
+    <t>30996088000104</t>
+  </si>
+  <si>
+    <t>VAGNER ALEXANDRE AMARAL RIBEIRO</t>
+  </si>
+  <si>
+    <t>36776404000119</t>
+  </si>
+  <si>
+    <t>ANTONIO ADEVALDO CARNEIRO DA SILVA</t>
+  </si>
+  <si>
+    <t>14387686000120</t>
+  </si>
+  <si>
+    <t>RENATO APARECIDO GOMES</t>
+  </si>
+  <si>
+    <t>18299482000198</t>
+  </si>
+  <si>
+    <t>J C - SURVEYORS - SERVICOS DE INSPECOES PORTUARIAS LTDA</t>
+  </si>
+  <si>
+    <t>11909608000150</t>
+  </si>
+  <si>
+    <t>MARCELO DE ANDRADE LTDA</t>
+  </si>
+  <si>
+    <t>37575672000135</t>
+  </si>
+  <si>
+    <t>ADILSON ORLANDO PEREIRA</t>
+  </si>
+  <si>
+    <t>14479466000126</t>
+  </si>
+  <si>
+    <t>NORTSYS SISTEMAS LTDA</t>
+  </si>
+  <si>
+    <t>13485667000173</t>
+  </si>
+  <si>
+    <t>A C DE OLIVEIRA CURSOS</t>
+  </si>
+  <si>
+    <t>54732936000136</t>
+  </si>
+  <si>
+    <t>S. P. MAGALHAES BUFFET</t>
+  </si>
+  <si>
+    <t>36677412000108</t>
+  </si>
+  <si>
+    <t>36.677.412 CELSO LEANDRO PERES GUEDES</t>
+  </si>
+  <si>
+    <t>39334730000164</t>
+  </si>
+  <si>
+    <t>LISCARLA BORGES</t>
+  </si>
+  <si>
+    <t>39584712000130</t>
+  </si>
+  <si>
+    <t>DONA PANCETA TORRESMO ARTESANAL LTDA</t>
+  </si>
+  <si>
+    <t>37486225000100</t>
+  </si>
+  <si>
+    <t>MARCELO FLAVIANO AMORIM</t>
+  </si>
+  <si>
+    <t>55927648000108</t>
+  </si>
+  <si>
+    <t>NEUROTREINO SOLUCOES COGNITIVAS LTDA</t>
+  </si>
+  <si>
+    <t>15236793000110</t>
+  </si>
+  <si>
+    <t>CENTRALIZA AMBIENTES PLANEJADOS LTDA</t>
+  </si>
+  <si>
+    <t>62547871000187</t>
+  </si>
+  <si>
+    <t>MINAS LOG LOCACAO DE VEICULOS E EQUIPAMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>15056135000146</t>
+  </si>
+  <si>
+    <t>MSB BEBIDAS LTDA</t>
+  </si>
+  <si>
+    <t>24383120000183</t>
+  </si>
+  <si>
+    <t>NEIDE APARECIDA DE JESUS DIAS ALMEIDA</t>
+  </si>
+  <si>
+    <t>33714260000188</t>
+  </si>
+  <si>
+    <t>JOSEILDO OZORIO CASSIANO</t>
+  </si>
+  <si>
+    <t>55666148000151</t>
+  </si>
+  <si>
+    <t>ORIGEM COMERCIO DE PRODUTOS ALIMENTICIOS LTDA</t>
+  </si>
+  <si>
+    <t>37482547000180</t>
+  </si>
+  <si>
+    <t>ELIEZER FARIA GABI</t>
+  </si>
+  <si>
+    <t>15577675000175</t>
+  </si>
+  <si>
+    <t>REPRESENTACOES MOREIRA LTDA</t>
+  </si>
+  <si>
+    <t>35285395000109</t>
+  </si>
+  <si>
+    <t>V &amp; V MONITORAMENTO DE ALARMES LTDA</t>
+  </si>
+  <si>
+    <t>63746196000188</t>
+  </si>
+  <si>
+    <t>LCT LTDA</t>
+  </si>
+  <si>
+    <t>35942617000291</t>
+  </si>
+  <si>
+    <t>CMS TRANSPORTES LOCACOES E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>29051529000116</t>
+  </si>
+  <si>
+    <t>29.051.529 SANAIANA SENA DA SILVA</t>
+  </si>
+  <si>
+    <t>62273369000125</t>
+  </si>
+  <si>
+    <t>M. V. DOS SANTOS TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>36213308000162</t>
+  </si>
+  <si>
+    <t>R TEIXEIRA ENGENHARIA CIVIL</t>
+  </si>
+  <si>
+    <t>28702928000137</t>
+  </si>
+  <si>
+    <t>KLISMANN JOSE PENTEADO HUBNER</t>
+  </si>
+  <si>
+    <t>33499992000100</t>
+  </si>
+  <si>
+    <t>PATIO CIDADE DAS PEDRAS LTDA</t>
+  </si>
+  <si>
+    <t>51029950000180</t>
+  </si>
+  <si>
+    <t>AVILA COMERCIO VAREJISTA DE VESTUARIO LTDA</t>
+  </si>
+  <si>
+    <t>57256999000151</t>
+  </si>
+  <si>
+    <t>KD2M SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>51441583000127</t>
+  </si>
+  <si>
+    <t>MS CONSULTORIA E PLANEJAMENTO EMPRESARIAL LTDA</t>
+  </si>
+  <si>
+    <t>29954826000171</t>
+  </si>
+  <si>
+    <t>N.C.A. FRETAMENTO E TURISMO LTDA</t>
+  </si>
+  <si>
+    <t>22511639000174</t>
+  </si>
+  <si>
+    <t>22.511.639 ROSANGELA BEATRIZ NUNES DA CUNHA</t>
+  </si>
+  <si>
+    <t>27306339000177</t>
+  </si>
+  <si>
+    <t>MASETTEC MAQUINAS LTDA</t>
+  </si>
+  <si>
+    <t>64328127000117</t>
+  </si>
+  <si>
+    <t>GUSTAVO ASSIS CASTRO SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>33641534000156</t>
+  </si>
+  <si>
+    <t>33.641.534 LUANA DE ALMEIDA AZEVEDO</t>
+  </si>
+  <si>
+    <t>64312456000170</t>
+  </si>
+  <si>
+    <t>PRISCILA DE OLIVEIRA SILVA PEIXOTO MANUTENCAO DE MAQUINAS LTDA</t>
+  </si>
+  <si>
+    <t>64327388000112</t>
+  </si>
+  <si>
+    <t>DANIELA EUSEBIO ASSESSORIA E CONSULTORIA CONTABIL LTDA</t>
+  </si>
+  <si>
+    <t>28715195000175</t>
+  </si>
+  <si>
+    <t>JOSE APARECIDO NOGUEIRA DE CASTRO</t>
+  </si>
+  <si>
+    <t>24188226000126</t>
+  </si>
+  <si>
+    <t>ANDERSON GOMES DA SILVA REFRIGERACAO LTDA</t>
+  </si>
+  <si>
+    <t>31433503000184</t>
+  </si>
+  <si>
+    <t>EMERSON DA SILVA XAVIER</t>
+  </si>
+  <si>
+    <t>19212783000103</t>
+  </si>
+  <si>
+    <t>HM TRANSPORTES LTDA.</t>
+  </si>
+  <si>
+    <t>34553962000190</t>
+  </si>
+  <si>
+    <t>VALENTIM MP LTDA</t>
+  </si>
+  <si>
+    <t>32946783000197</t>
+  </si>
+  <si>
+    <t>ANDREIA MARONN SAUSEN</t>
+  </si>
+  <si>
+    <t>34917508000170</t>
+  </si>
+  <si>
+    <t>D.CLARA EVENTOS LTDA</t>
+  </si>
+  <si>
+    <t>62992278000140</t>
+  </si>
+  <si>
+    <t>FERREIRA PORTELLA LTDA</t>
+  </si>
+  <si>
+    <t>63009986000180</t>
+  </si>
+  <si>
+    <t>INDUSTRIA DE PLASTICOS PARA CALCADOS POWEER LTDA</t>
+  </si>
+  <si>
+    <t>26721499000110</t>
+  </si>
+  <si>
+    <t>ADEMILSON PIONELLI SERVICOS AGRICOLAS</t>
+  </si>
+  <si>
+    <t>64312780000198</t>
+  </si>
+  <si>
+    <t>J V COSTA DE PAULA</t>
+  </si>
+  <si>
+    <t>64248161000181</t>
+  </si>
+  <si>
+    <t>PESSOA AIRES SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>63796861000148</t>
+  </si>
+  <si>
+    <t>A2S SOLUCOES INTEGRADAS LTDA</t>
+  </si>
+  <si>
+    <t>32119168000107</t>
+  </si>
+  <si>
+    <t>ORLANDO BALDUINO DE FREITAS</t>
+  </si>
+  <si>
+    <t>64313843000120</t>
+  </si>
+  <si>
+    <t>USINA POLIMIX CONCRETO BR INOVA SIMPLES (I.S.)</t>
+  </si>
+  <si>
+    <t>54799997000200</t>
+  </si>
+  <si>
+    <t>CAMPO FORTE IRRIGACAO LTDA</t>
+  </si>
+  <si>
+    <t>20184417000169</t>
+  </si>
+  <si>
+    <t>ADAIAS C DE C SILVA</t>
+  </si>
+  <si>
+    <t>24925009000171</t>
+  </si>
+  <si>
+    <t>J A B DE LIMA MECANICA</t>
+  </si>
+  <si>
+    <t>37752564000190</t>
+  </si>
+  <si>
+    <t>LEANDRA LYSLE GARCIA LIGUORI LTDA</t>
+  </si>
+  <si>
+    <t>36350412000107</t>
+  </si>
+  <si>
+    <t>G D BUENO COMERCIO DE MILHO VERDE</t>
+  </si>
+  <si>
+    <t>28622459000146</t>
+  </si>
+  <si>
+    <t>CAMILA NATALIA RODRIGUES MARTINS</t>
+  </si>
+  <si>
+    <t>63654795000171</t>
+  </si>
+  <si>
+    <t>ALESSANDRO SPINELLI RABELO</t>
+  </si>
+  <si>
+    <t>11878104000110</t>
+  </si>
+  <si>
+    <t>AJJ MONTADORA  INSTALADORA BELFORD LTDA</t>
+  </si>
+  <si>
+    <t>59182036000186</t>
+  </si>
+  <si>
+    <t>CR SERVICOS E LOCACOES LTDA</t>
+  </si>
+  <si>
+    <t>29972507000199</t>
+  </si>
+  <si>
+    <t>CH MOVEIS LTDA</t>
+  </si>
+  <si>
+    <t>51002586000164</t>
+  </si>
+  <si>
+    <t>G  A CONSTRUTORA LTDA</t>
+  </si>
+  <si>
+    <t>39822221000180</t>
+  </si>
+  <si>
+    <t>SANTOS AMORIM ESTACIONAMENTO LTDA</t>
+  </si>
+  <si>
+    <t>63190932000164</t>
+  </si>
+  <si>
+    <t>JAQUELINE A M ARBAGE</t>
+  </si>
+  <si>
+    <t>63204415000105</t>
+  </si>
+  <si>
+    <t>HEBERT FREIRE SANTOS HEBERT FREIRE SANTOS</t>
+  </si>
+  <si>
+    <t>Procuracao com poderes para abrir e movimentar contas, pois identificamos que a representacao da sua empresa deve ser em conjunto pelos representantes. O documento deve ser assinado pelos representantes legais nomeados no contrato social, assinada digitalmente GOV.br ou procuracao publica. Em caso de assinatura digital, devera ser encaminhado o documento em formato PDF, para validacao das assinaturas e protocolo de autenticidade.</t>
+  </si>
+  <si>
+    <t>Contrato Social atualizado e registrado no orgao competente</t>
   </si>
 </sst>
 </file>
@@ -2140,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A45A88-3D17-4433-986A-11075963C36F}">
   <dimension ref="A1:G1330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
-      <selection activeCell="F274" sqref="F274"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3638,7 +4235,7 @@
         <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -4261,6 +4858,9 @@
       <c r="F92" t="s">
         <v>575</v>
       </c>
+      <c r="G92" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
@@ -5107,7 +5707,7 @@
         <v>8</v>
       </c>
       <c r="F129" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -5638,6 +6238,9 @@
       <c r="F152" t="s">
         <v>575</v>
       </c>
+      <c r="G152" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
@@ -5817,7 +6420,7 @@
         <v>8</v>
       </c>
       <c r="F160" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G160">
         <v>0</v>
@@ -5886,7 +6489,7 @@
         <v>12</v>
       </c>
       <c r="F163" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G163">
         <v>0</v>
@@ -6139,7 +6742,7 @@
         <v>8</v>
       </c>
       <c r="F174" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G174">
         <v>0</v>
@@ -6415,7 +7018,7 @@
         <v>7</v>
       </c>
       <c r="F186" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G186">
         <v>0</v>
@@ -6461,7 +7064,7 @@
         <v>7</v>
       </c>
       <c r="F188" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G188">
         <v>0</v>
@@ -6486,6 +7089,9 @@
       <c r="F189" t="s">
         <v>575</v>
       </c>
+      <c r="G189" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
@@ -6619,7 +7225,7 @@
         <v>8</v>
       </c>
       <c r="F195" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -6688,7 +7294,7 @@
         <v>8</v>
       </c>
       <c r="F198" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G198">
         <v>0</v>
@@ -6711,7 +7317,7 @@
         <v>8</v>
       </c>
       <c r="F199" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G199">
         <v>0</v>
@@ -6872,10 +7478,10 @@
         <v>8</v>
       </c>
       <c r="F206" t="s">
-        <v>576</v>
-      </c>
-      <c r="G206">
-        <v>0</v>
+        <v>574</v>
+      </c>
+      <c r="G206" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -7150,6 +7756,9 @@
       <c r="F218" t="s">
         <v>575</v>
       </c>
+      <c r="G218" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
@@ -7329,7 +7938,7 @@
         <v>7</v>
       </c>
       <c r="F226" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G226">
         <v>0</v>
@@ -7490,7 +8099,7 @@
         <v>8</v>
       </c>
       <c r="F233" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G233">
         <v>0</v>
@@ -7513,7 +8122,10 @@
         <v>21</v>
       </c>
       <c r="F234" t="s">
-        <v>576</v>
+        <v>573</v>
+      </c>
+      <c r="G234">
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -7533,7 +8145,7 @@
         <v>8</v>
       </c>
       <c r="F235" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G235">
         <v>0</v>
@@ -7671,7 +8283,7 @@
         <v>8</v>
       </c>
       <c r="F241" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G241">
         <v>0</v>
@@ -7740,7 +8352,7 @@
         <v>7</v>
       </c>
       <c r="F244" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G244">
         <v>0</v>
@@ -8110,9 +8722,6 @@
       <c r="F260" t="s">
         <v>572</v>
       </c>
-      <c r="G260">
-        <v>0</v>
-      </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
@@ -8414,336 +9023,2290 @@
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A274" s="1"/>
+      <c r="A274" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B274" t="s">
+        <v>577</v>
+      </c>
+      <c r="C274" t="s">
+        <v>578</v>
+      </c>
+      <c r="D274" t="s">
+        <v>18</v>
+      </c>
+      <c r="E274" t="s">
+        <v>19</v>
+      </c>
+      <c r="F274" t="s">
+        <v>572</v>
+      </c>
+      <c r="G274">
+        <v>0</v>
+      </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A275" s="1"/>
+      <c r="A275" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B275" t="s">
+        <v>579</v>
+      </c>
+      <c r="C275" t="s">
+        <v>580</v>
+      </c>
+      <c r="D275" t="s">
+        <v>18</v>
+      </c>
+      <c r="E275" t="s">
+        <v>19</v>
+      </c>
+      <c r="F275" t="s">
+        <v>572</v>
+      </c>
+      <c r="G275">
+        <v>0</v>
+      </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A276" s="1"/>
+      <c r="A276" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B276" t="s">
+        <v>581</v>
+      </c>
+      <c r="C276" t="s">
+        <v>582</v>
+      </c>
+      <c r="D276" t="s">
+        <v>18</v>
+      </c>
+      <c r="E276" t="s">
+        <v>19</v>
+      </c>
+      <c r="F276" t="s">
+        <v>572</v>
+      </c>
+      <c r="G276">
+        <v>0</v>
+      </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277" s="1"/>
+      <c r="A277" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B277" t="s">
+        <v>583</v>
+      </c>
+      <c r="C277" t="s">
+        <v>584</v>
+      </c>
+      <c r="D277" t="s">
+        <v>134</v>
+      </c>
+      <c r="E277" t="s">
+        <v>8</v>
+      </c>
+      <c r="F277" t="s">
+        <v>571</v>
+      </c>
+      <c r="G277">
+        <v>0</v>
+      </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="1"/>
+      <c r="A278" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B278" t="s">
+        <v>585</v>
+      </c>
+      <c r="C278" t="s">
+        <v>586</v>
+      </c>
+      <c r="D278" t="s">
+        <v>131</v>
+      </c>
+      <c r="E278" t="s">
+        <v>8</v>
+      </c>
+      <c r="F278" t="s">
+        <v>576</v>
+      </c>
+      <c r="G278" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A279" s="1"/>
+      <c r="A279" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B279" t="s">
+        <v>587</v>
+      </c>
+      <c r="C279" t="s">
+        <v>588</v>
+      </c>
+      <c r="D279" t="s">
+        <v>154</v>
+      </c>
+      <c r="E279" t="s">
+        <v>12</v>
+      </c>
+      <c r="F279" t="s">
+        <v>572</v>
+      </c>
+      <c r="G279">
+        <v>0</v>
+      </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A280" s="1"/>
+      <c r="A280" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B280" t="s">
+        <v>589</v>
+      </c>
+      <c r="C280" t="s">
+        <v>590</v>
+      </c>
+      <c r="D280" t="s">
+        <v>22</v>
+      </c>
+      <c r="E280" t="s">
+        <v>8</v>
+      </c>
+      <c r="F280" t="s">
+        <v>576</v>
+      </c>
+      <c r="G280">
+        <v>0</v>
+      </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A281" s="1"/>
+      <c r="A281" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B281" t="s">
+        <v>591</v>
+      </c>
+      <c r="C281" t="s">
+        <v>592</v>
+      </c>
+      <c r="D281" t="s">
+        <v>209</v>
+      </c>
+      <c r="E281" t="s">
+        <v>7</v>
+      </c>
+      <c r="F281" t="s">
+        <v>572</v>
+      </c>
+      <c r="G281">
+        <v>0</v>
+      </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282" s="1"/>
+      <c r="A282" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B282" t="s">
+        <v>593</v>
+      </c>
+      <c r="C282" t="s">
+        <v>594</v>
+      </c>
+      <c r="D282" t="s">
+        <v>10</v>
+      </c>
+      <c r="E282" t="s">
+        <v>7</v>
+      </c>
+      <c r="F282" t="s">
+        <v>572</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
+      </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A283" s="1"/>
+      <c r="A283" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B283" t="s">
+        <v>595</v>
+      </c>
+      <c r="C283" t="s">
+        <v>596</v>
+      </c>
+      <c r="D283" t="s">
+        <v>17</v>
+      </c>
+      <c r="E283" t="s">
+        <v>8</v>
+      </c>
+      <c r="F283" t="s">
+        <v>572</v>
+      </c>
+      <c r="G283">
+        <v>0</v>
+      </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A284" s="1"/>
+      <c r="A284" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B284" t="s">
+        <v>597</v>
+      </c>
+      <c r="C284" t="s">
+        <v>598</v>
+      </c>
+      <c r="D284" t="s">
+        <v>16</v>
+      </c>
+      <c r="E284" t="s">
+        <v>8</v>
+      </c>
+      <c r="F284" t="s">
+        <v>571</v>
+      </c>
+      <c r="G284">
+        <v>0</v>
+      </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" s="1"/>
+      <c r="A285" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B285" t="s">
+        <v>599</v>
+      </c>
+      <c r="C285" t="s">
+        <v>600</v>
+      </c>
+      <c r="D285" t="s">
+        <v>14</v>
+      </c>
+      <c r="E285" t="s">
+        <v>8</v>
+      </c>
+      <c r="F285" t="s">
+        <v>576</v>
+      </c>
+      <c r="G285">
+        <v>0</v>
+      </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="1"/>
+      <c r="A286" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B286" t="s">
+        <v>601</v>
+      </c>
+      <c r="C286" t="s">
+        <v>602</v>
+      </c>
+      <c r="D286" t="s">
+        <v>131</v>
+      </c>
+      <c r="E286" t="s">
+        <v>8</v>
+      </c>
+      <c r="F286" t="s">
+        <v>572</v>
+      </c>
+      <c r="G286">
+        <v>0</v>
+      </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" s="1"/>
+      <c r="A287" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B287" t="s">
+        <v>603</v>
+      </c>
+      <c r="C287" t="s">
+        <v>604</v>
+      </c>
+      <c r="D287" t="s">
+        <v>13</v>
+      </c>
+      <c r="E287" t="s">
+        <v>8</v>
+      </c>
+      <c r="F287" t="s">
+        <v>572</v>
+      </c>
+      <c r="G287">
+        <v>0</v>
+      </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A288" s="1"/>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" s="1"/>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="1"/>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="1"/>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="1"/>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="1"/>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="1"/>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" s="1"/>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="1"/>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="1"/>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" s="1"/>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="1"/>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="1"/>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="1"/>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="1"/>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="1"/>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="1"/>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="1"/>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="1"/>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="1"/>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" s="1"/>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="1"/>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="1"/>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="1"/>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="1"/>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="1"/>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="1"/>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="1"/>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="1"/>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="1"/>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" s="1"/>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="1"/>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="1"/>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="1"/>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="1"/>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="1"/>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="1"/>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" s="1"/>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="1"/>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="1"/>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="1"/>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="1"/>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="1"/>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="1"/>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="1"/>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" s="1"/>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="1"/>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="1"/>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="1"/>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="1"/>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="1"/>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" s="1"/>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="1"/>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="1"/>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="1"/>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="1"/>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="1"/>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="1"/>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" s="1"/>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="1"/>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="1"/>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" s="1"/>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="1"/>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="1"/>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="1"/>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="1"/>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="1"/>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" s="1"/>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="1"/>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="1"/>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" s="1"/>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="1"/>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" s="1"/>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="1"/>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="1"/>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="1"/>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="1"/>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="1"/>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="1"/>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="1"/>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" s="1"/>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="1"/>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="1"/>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="1"/>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B288" t="s">
+        <v>605</v>
+      </c>
+      <c r="C288" t="s">
+        <v>606</v>
+      </c>
+      <c r="D288" t="s">
+        <v>116</v>
+      </c>
+      <c r="E288" t="s">
+        <v>8</v>
+      </c>
+      <c r="F288" t="s">
+        <v>572</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B289" t="s">
+        <v>607</v>
+      </c>
+      <c r="C289" t="s">
+        <v>608</v>
+      </c>
+      <c r="D289" t="s">
+        <v>10</v>
+      </c>
+      <c r="E289" t="s">
+        <v>7</v>
+      </c>
+      <c r="F289" t="s">
+        <v>609</v>
+      </c>
+      <c r="G289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B290" t="s">
+        <v>610</v>
+      </c>
+      <c r="C290" t="s">
+        <v>611</v>
+      </c>
+      <c r="D290" t="s">
+        <v>16</v>
+      </c>
+      <c r="E290" t="s">
+        <v>8</v>
+      </c>
+      <c r="F290" t="s">
+        <v>572</v>
+      </c>
+      <c r="G290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B291" t="s">
+        <v>612</v>
+      </c>
+      <c r="C291" t="s">
+        <v>613</v>
+      </c>
+      <c r="D291" t="s">
+        <v>134</v>
+      </c>
+      <c r="E291" t="s">
+        <v>20</v>
+      </c>
+      <c r="F291" t="s">
+        <v>572</v>
+      </c>
+      <c r="G291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B292" t="s">
+        <v>614</v>
+      </c>
+      <c r="C292" t="s">
+        <v>615</v>
+      </c>
+      <c r="D292" t="s">
+        <v>17</v>
+      </c>
+      <c r="E292" t="s">
+        <v>8</v>
+      </c>
+      <c r="F292" t="s">
+        <v>572</v>
+      </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B293" t="s">
+        <v>616</v>
+      </c>
+      <c r="C293" t="s">
+        <v>617</v>
+      </c>
+      <c r="D293" t="s">
+        <v>13</v>
+      </c>
+      <c r="E293" t="s">
+        <v>8</v>
+      </c>
+      <c r="F293" t="s">
+        <v>576</v>
+      </c>
+      <c r="G293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B294" t="s">
+        <v>618</v>
+      </c>
+      <c r="C294" t="s">
+        <v>619</v>
+      </c>
+      <c r="D294" t="s">
+        <v>13</v>
+      </c>
+      <c r="E294" t="s">
+        <v>8</v>
+      </c>
+      <c r="F294" t="s">
+        <v>572</v>
+      </c>
+      <c r="G294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B295" t="s">
+        <v>620</v>
+      </c>
+      <c r="C295" t="s">
+        <v>621</v>
+      </c>
+      <c r="D295" t="s">
+        <v>17</v>
+      </c>
+      <c r="E295" t="s">
+        <v>8</v>
+      </c>
+      <c r="F295" t="s">
+        <v>572</v>
+      </c>
+      <c r="G295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B296" t="s">
+        <v>622</v>
+      </c>
+      <c r="C296" t="s">
+        <v>623</v>
+      </c>
+      <c r="D296" t="s">
+        <v>16</v>
+      </c>
+      <c r="E296" t="s">
+        <v>8</v>
+      </c>
+      <c r="F296" t="s">
+        <v>571</v>
+      </c>
+      <c r="G296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B297" t="s">
+        <v>624</v>
+      </c>
+      <c r="C297" t="s">
+        <v>625</v>
+      </c>
+      <c r="D297" t="s">
+        <v>14</v>
+      </c>
+      <c r="E297" t="s">
+        <v>8</v>
+      </c>
+      <c r="F297" t="s">
+        <v>576</v>
+      </c>
+      <c r="G297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B298" t="s">
+        <v>626</v>
+      </c>
+      <c r="C298" t="s">
+        <v>627</v>
+      </c>
+      <c r="D298" t="s">
+        <v>22</v>
+      </c>
+      <c r="E298" t="s">
+        <v>8</v>
+      </c>
+      <c r="F298" t="s">
+        <v>572</v>
+      </c>
+      <c r="G298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B299" t="s">
+        <v>628</v>
+      </c>
+      <c r="C299" t="s">
+        <v>629</v>
+      </c>
+      <c r="D299" t="s">
+        <v>209</v>
+      </c>
+      <c r="E299" t="s">
+        <v>12</v>
+      </c>
+      <c r="F299" t="s">
+        <v>572</v>
+      </c>
+      <c r="G299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B300" t="s">
+        <v>630</v>
+      </c>
+      <c r="C300" t="s">
+        <v>631</v>
+      </c>
+      <c r="D300" t="s">
+        <v>13</v>
+      </c>
+      <c r="E300" t="s">
+        <v>20</v>
+      </c>
+      <c r="F300" t="s">
+        <v>572</v>
+      </c>
+      <c r="G300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B301" t="s">
+        <v>632</v>
+      </c>
+      <c r="C301" t="s">
+        <v>633</v>
+      </c>
+      <c r="D301" t="s">
+        <v>10</v>
+      </c>
+      <c r="E301" t="s">
+        <v>8</v>
+      </c>
+      <c r="F301" t="s">
+        <v>572</v>
+      </c>
+      <c r="G301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B302" t="s">
+        <v>634</v>
+      </c>
+      <c r="C302" t="s">
+        <v>635</v>
+      </c>
+      <c r="D302" t="s">
+        <v>134</v>
+      </c>
+      <c r="E302" t="s">
+        <v>8</v>
+      </c>
+      <c r="F302" t="s">
+        <v>572</v>
+      </c>
+      <c r="G302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B303" t="s">
+        <v>636</v>
+      </c>
+      <c r="C303" t="s">
+        <v>637</v>
+      </c>
+      <c r="D303" t="s">
+        <v>22</v>
+      </c>
+      <c r="E303" t="s">
+        <v>8</v>
+      </c>
+      <c r="F303" t="s">
+        <v>572</v>
+      </c>
+      <c r="G303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B304" t="s">
+        <v>638</v>
+      </c>
+      <c r="C304" t="s">
+        <v>639</v>
+      </c>
+      <c r="D304" t="s">
+        <v>6</v>
+      </c>
+      <c r="E304" t="s">
+        <v>8</v>
+      </c>
+      <c r="F304" t="s">
+        <v>572</v>
+      </c>
+      <c r="G304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B305" t="s">
+        <v>640</v>
+      </c>
+      <c r="C305" t="s">
+        <v>641</v>
+      </c>
+      <c r="D305" t="s">
+        <v>17</v>
+      </c>
+      <c r="E305" t="s">
+        <v>8</v>
+      </c>
+      <c r="F305" t="s">
+        <v>572</v>
+      </c>
+      <c r="G305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B306" t="s">
+        <v>642</v>
+      </c>
+      <c r="C306" t="s">
+        <v>643</v>
+      </c>
+      <c r="D306" t="s">
+        <v>237</v>
+      </c>
+      <c r="E306" t="s">
+        <v>7</v>
+      </c>
+      <c r="F306" t="s">
+        <v>576</v>
+      </c>
+      <c r="G306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B307" t="s">
+        <v>644</v>
+      </c>
+      <c r="C307" t="s">
+        <v>645</v>
+      </c>
+      <c r="D307" t="s">
+        <v>16</v>
+      </c>
+      <c r="E307" t="s">
+        <v>8</v>
+      </c>
+      <c r="F307" t="s">
+        <v>572</v>
+      </c>
+      <c r="G307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B308" t="s">
+        <v>646</v>
+      </c>
+      <c r="C308" t="s">
+        <v>647</v>
+      </c>
+      <c r="D308" t="s">
+        <v>13</v>
+      </c>
+      <c r="E308" t="s">
+        <v>8</v>
+      </c>
+      <c r="F308" t="s">
+        <v>572</v>
+      </c>
+      <c r="G308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B309" t="s">
+        <v>648</v>
+      </c>
+      <c r="C309" t="s">
+        <v>649</v>
+      </c>
+      <c r="D309" t="s">
+        <v>113</v>
+      </c>
+      <c r="E309" t="s">
+        <v>8</v>
+      </c>
+      <c r="F309" t="s">
+        <v>576</v>
+      </c>
+      <c r="G309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B310" t="s">
+        <v>650</v>
+      </c>
+      <c r="C310" t="s">
+        <v>651</v>
+      </c>
+      <c r="D310" t="s">
+        <v>237</v>
+      </c>
+      <c r="E310" t="s">
+        <v>8</v>
+      </c>
+      <c r="F310" t="s">
+        <v>572</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B311" t="s">
+        <v>652</v>
+      </c>
+      <c r="C311" t="s">
+        <v>653</v>
+      </c>
+      <c r="D311" t="s">
+        <v>16</v>
+      </c>
+      <c r="E311" t="s">
+        <v>8</v>
+      </c>
+      <c r="F311" t="s">
+        <v>572</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B312" t="s">
+        <v>654</v>
+      </c>
+      <c r="C312" t="s">
+        <v>655</v>
+      </c>
+      <c r="D312" t="s">
+        <v>44</v>
+      </c>
+      <c r="E312" t="s">
+        <v>8</v>
+      </c>
+      <c r="F312" t="s">
+        <v>572</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B313" t="s">
+        <v>656</v>
+      </c>
+      <c r="C313" t="s">
+        <v>657</v>
+      </c>
+      <c r="D313" t="s">
+        <v>22</v>
+      </c>
+      <c r="E313" t="s">
+        <v>8</v>
+      </c>
+      <c r="F313" t="s">
+        <v>572</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B314" t="s">
+        <v>658</v>
+      </c>
+      <c r="C314" t="s">
+        <v>659</v>
+      </c>
+      <c r="D314" t="s">
+        <v>15</v>
+      </c>
+      <c r="E314" t="s">
+        <v>12</v>
+      </c>
+      <c r="F314" t="s">
+        <v>572</v>
+      </c>
+      <c r="G314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B315" t="s">
+        <v>660</v>
+      </c>
+      <c r="C315" t="s">
+        <v>661</v>
+      </c>
+      <c r="D315" t="s">
+        <v>15</v>
+      </c>
+      <c r="E315" t="s">
+        <v>12</v>
+      </c>
+      <c r="F315" t="s">
+        <v>572</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B316" t="s">
+        <v>662</v>
+      </c>
+      <c r="C316" t="s">
+        <v>663</v>
+      </c>
+      <c r="D316" t="s">
+        <v>6</v>
+      </c>
+      <c r="E316" t="s">
+        <v>8</v>
+      </c>
+      <c r="F316" t="s">
+        <v>572</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B317" t="s">
+        <v>664</v>
+      </c>
+      <c r="C317" t="s">
+        <v>665</v>
+      </c>
+      <c r="D317" t="s">
+        <v>14</v>
+      </c>
+      <c r="E317" t="s">
+        <v>8</v>
+      </c>
+      <c r="F317" t="s">
+        <v>572</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B318" t="s">
+        <v>666</v>
+      </c>
+      <c r="C318" t="s">
+        <v>667</v>
+      </c>
+      <c r="D318" t="s">
+        <v>131</v>
+      </c>
+      <c r="E318" t="s">
+        <v>8</v>
+      </c>
+      <c r="F318" t="s">
+        <v>572</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B319" t="s">
+        <v>668</v>
+      </c>
+      <c r="C319" t="s">
+        <v>669</v>
+      </c>
+      <c r="D319" t="s">
+        <v>22</v>
+      </c>
+      <c r="E319" t="s">
+        <v>8</v>
+      </c>
+      <c r="F319" t="s">
+        <v>574</v>
+      </c>
+      <c r="G319" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B320" t="s">
+        <v>670</v>
+      </c>
+      <c r="C320" t="s">
+        <v>671</v>
+      </c>
+      <c r="D320" t="s">
+        <v>134</v>
+      </c>
+      <c r="E320" t="s">
+        <v>8</v>
+      </c>
+      <c r="F320" t="s">
+        <v>572</v>
+      </c>
+      <c r="G320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A321" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B321" t="s">
+        <v>672</v>
+      </c>
+      <c r="C321" t="s">
+        <v>673</v>
+      </c>
+      <c r="D321" t="s">
+        <v>22</v>
+      </c>
+      <c r="E321" t="s">
+        <v>8</v>
+      </c>
+      <c r="F321" t="s">
+        <v>576</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A322" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B322" t="s">
+        <v>674</v>
+      </c>
+      <c r="C322" t="s">
+        <v>675</v>
+      </c>
+      <c r="D322" t="s">
+        <v>131</v>
+      </c>
+      <c r="E322" t="s">
+        <v>8</v>
+      </c>
+      <c r="F322" t="s">
+        <v>571</v>
+      </c>
+      <c r="G322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A323" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B323" t="s">
+        <v>676</v>
+      </c>
+      <c r="C323" t="s">
+        <v>677</v>
+      </c>
+      <c r="D323" t="s">
+        <v>209</v>
+      </c>
+      <c r="E323" t="s">
+        <v>8</v>
+      </c>
+      <c r="F323" t="s">
+        <v>576</v>
+      </c>
+      <c r="G323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A324" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B324" t="s">
+        <v>678</v>
+      </c>
+      <c r="C324" t="s">
+        <v>679</v>
+      </c>
+      <c r="D324" t="s">
+        <v>22</v>
+      </c>
+      <c r="E324" t="s">
+        <v>8</v>
+      </c>
+      <c r="F324" t="s">
+        <v>572</v>
+      </c>
+      <c r="G324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A325" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B325" t="s">
+        <v>680</v>
+      </c>
+      <c r="C325" t="s">
+        <v>681</v>
+      </c>
+      <c r="D325" t="s">
+        <v>9</v>
+      </c>
+      <c r="E325" t="s">
+        <v>8</v>
+      </c>
+      <c r="F325" t="s">
+        <v>572</v>
+      </c>
+      <c r="G325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A326" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B326" t="s">
+        <v>682</v>
+      </c>
+      <c r="C326" t="s">
+        <v>683</v>
+      </c>
+      <c r="D326" t="s">
+        <v>237</v>
+      </c>
+      <c r="E326" t="s">
+        <v>8</v>
+      </c>
+      <c r="F326" t="s">
+        <v>571</v>
+      </c>
+      <c r="G326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A327" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B327" t="s">
+        <v>684</v>
+      </c>
+      <c r="C327" t="s">
+        <v>685</v>
+      </c>
+      <c r="D327" t="s">
+        <v>13</v>
+      </c>
+      <c r="E327" t="s">
+        <v>8</v>
+      </c>
+      <c r="F327" t="s">
+        <v>576</v>
+      </c>
+      <c r="G327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A328" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B328" t="s">
+        <v>686</v>
+      </c>
+      <c r="C328" t="s">
+        <v>687</v>
+      </c>
+      <c r="D328" t="s">
+        <v>131</v>
+      </c>
+      <c r="E328" t="s">
+        <v>8</v>
+      </c>
+      <c r="F328" t="s">
+        <v>572</v>
+      </c>
+      <c r="G328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B329" t="s">
+        <v>688</v>
+      </c>
+      <c r="C329" t="s">
+        <v>689</v>
+      </c>
+      <c r="D329" t="s">
+        <v>11</v>
+      </c>
+      <c r="E329" t="s">
+        <v>8</v>
+      </c>
+      <c r="F329" t="s">
+        <v>576</v>
+      </c>
+      <c r="G329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B330" t="s">
+        <v>690</v>
+      </c>
+      <c r="C330" t="s">
+        <v>691</v>
+      </c>
+      <c r="D330" t="s">
+        <v>134</v>
+      </c>
+      <c r="E330" t="s">
+        <v>8</v>
+      </c>
+      <c r="F330" t="s">
+        <v>576</v>
+      </c>
+      <c r="G330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B331" t="s">
+        <v>692</v>
+      </c>
+      <c r="C331" t="s">
+        <v>693</v>
+      </c>
+      <c r="D331" t="s">
+        <v>154</v>
+      </c>
+      <c r="E331" t="s">
+        <v>12</v>
+      </c>
+      <c r="F331" t="s">
+        <v>572</v>
+      </c>
+      <c r="G331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B332" t="s">
+        <v>694</v>
+      </c>
+      <c r="C332" t="s">
+        <v>695</v>
+      </c>
+      <c r="D332" t="s">
+        <v>10</v>
+      </c>
+      <c r="E332" t="s">
+        <v>8</v>
+      </c>
+      <c r="F332" t="s">
+        <v>576</v>
+      </c>
+      <c r="G332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B333" t="s">
+        <v>696</v>
+      </c>
+      <c r="C333" t="s">
+        <v>697</v>
+      </c>
+      <c r="D333" t="s">
+        <v>23</v>
+      </c>
+      <c r="E333" t="s">
+        <v>8</v>
+      </c>
+      <c r="F333" t="s">
+        <v>572</v>
+      </c>
+      <c r="G333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B334" t="s">
+        <v>698</v>
+      </c>
+      <c r="C334" t="s">
+        <v>699</v>
+      </c>
+      <c r="D334" t="s">
+        <v>14</v>
+      </c>
+      <c r="E334" t="s">
+        <v>8</v>
+      </c>
+      <c r="F334" t="s">
+        <v>572</v>
+      </c>
+      <c r="G334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B335" t="s">
+        <v>700</v>
+      </c>
+      <c r="C335" t="s">
+        <v>701</v>
+      </c>
+      <c r="D335" t="s">
+        <v>15</v>
+      </c>
+      <c r="E335" t="s">
+        <v>12</v>
+      </c>
+      <c r="F335" t="s">
+        <v>572</v>
+      </c>
+      <c r="G335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B336" t="s">
+        <v>702</v>
+      </c>
+      <c r="C336" t="s">
+        <v>703</v>
+      </c>
+      <c r="D336" t="s">
+        <v>16</v>
+      </c>
+      <c r="E336" t="s">
+        <v>8</v>
+      </c>
+      <c r="F336" t="s">
+        <v>572</v>
+      </c>
+      <c r="G336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B337" t="s">
+        <v>704</v>
+      </c>
+      <c r="C337" t="s">
+        <v>705</v>
+      </c>
+      <c r="D337" t="s">
+        <v>209</v>
+      </c>
+      <c r="E337" t="s">
+        <v>8</v>
+      </c>
+      <c r="F337" t="s">
+        <v>572</v>
+      </c>
+      <c r="G337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B338" t="s">
+        <v>706</v>
+      </c>
+      <c r="C338" t="s">
+        <v>707</v>
+      </c>
+      <c r="D338" t="s">
+        <v>23</v>
+      </c>
+      <c r="E338" t="s">
+        <v>8</v>
+      </c>
+      <c r="F338" t="s">
+        <v>572</v>
+      </c>
+      <c r="G338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B339" t="s">
+        <v>708</v>
+      </c>
+      <c r="C339" t="s">
+        <v>709</v>
+      </c>
+      <c r="D339" t="s">
+        <v>237</v>
+      </c>
+      <c r="E339" t="s">
+        <v>12</v>
+      </c>
+      <c r="F339" t="s">
+        <v>572</v>
+      </c>
+      <c r="G339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B340" t="s">
+        <v>710</v>
+      </c>
+      <c r="C340" t="s">
+        <v>711</v>
+      </c>
+      <c r="D340" t="s">
+        <v>116</v>
+      </c>
+      <c r="E340" t="s">
+        <v>8</v>
+      </c>
+      <c r="F340" t="s">
+        <v>572</v>
+      </c>
+      <c r="G340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A341" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B341" t="s">
+        <v>712</v>
+      </c>
+      <c r="C341" t="s">
+        <v>713</v>
+      </c>
+      <c r="D341" t="s">
+        <v>15</v>
+      </c>
+      <c r="E341" t="s">
+        <v>12</v>
+      </c>
+      <c r="F341" t="s">
+        <v>572</v>
+      </c>
+      <c r="G341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B342" t="s">
+        <v>714</v>
+      </c>
+      <c r="C342" t="s">
+        <v>715</v>
+      </c>
+      <c r="D342" t="s">
+        <v>154</v>
+      </c>
+      <c r="E342" t="s">
+        <v>12</v>
+      </c>
+      <c r="F342" t="s">
+        <v>576</v>
+      </c>
+      <c r="G342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A343" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B343" t="s">
+        <v>716</v>
+      </c>
+      <c r="C343" t="s">
+        <v>717</v>
+      </c>
+      <c r="D343" t="s">
+        <v>13</v>
+      </c>
+      <c r="E343" t="s">
+        <v>8</v>
+      </c>
+      <c r="F343" t="s">
+        <v>572</v>
+      </c>
+      <c r="G343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A344" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B344" t="s">
+        <v>718</v>
+      </c>
+      <c r="C344" t="s">
+        <v>719</v>
+      </c>
+      <c r="D344" t="s">
+        <v>16</v>
+      </c>
+      <c r="E344" t="s">
+        <v>8</v>
+      </c>
+      <c r="F344" t="s">
+        <v>572</v>
+      </c>
+      <c r="G344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A345" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B345" t="s">
+        <v>720</v>
+      </c>
+      <c r="C345" t="s">
+        <v>721</v>
+      </c>
+      <c r="D345" t="s">
+        <v>209</v>
+      </c>
+      <c r="E345" t="s">
+        <v>8</v>
+      </c>
+      <c r="F345" t="s">
+        <v>576</v>
+      </c>
+      <c r="G345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A346" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B346" t="s">
+        <v>722</v>
+      </c>
+      <c r="C346" t="s">
+        <v>723</v>
+      </c>
+      <c r="D346" t="s">
+        <v>22</v>
+      </c>
+      <c r="E346" t="s">
+        <v>8</v>
+      </c>
+      <c r="F346" t="s">
+        <v>576</v>
+      </c>
+      <c r="G346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A347" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B347" t="s">
+        <v>724</v>
+      </c>
+      <c r="C347" t="s">
+        <v>725</v>
+      </c>
+      <c r="D347" t="s">
+        <v>116</v>
+      </c>
+      <c r="E347" t="s">
+        <v>8</v>
+      </c>
+      <c r="F347" t="s">
+        <v>572</v>
+      </c>
+      <c r="G347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A348" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B348" t="s">
+        <v>726</v>
+      </c>
+      <c r="C348" t="s">
+        <v>727</v>
+      </c>
+      <c r="D348" t="s">
+        <v>22</v>
+      </c>
+      <c r="E348" t="s">
+        <v>8</v>
+      </c>
+      <c r="F348" t="s">
+        <v>572</v>
+      </c>
+      <c r="G348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A349" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B349" t="s">
+        <v>728</v>
+      </c>
+      <c r="C349" t="s">
+        <v>729</v>
+      </c>
+      <c r="D349" t="s">
+        <v>14</v>
+      </c>
+      <c r="E349" t="s">
+        <v>8</v>
+      </c>
+      <c r="F349" t="s">
+        <v>576</v>
+      </c>
+      <c r="G349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A350" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B350" t="s">
+        <v>730</v>
+      </c>
+      <c r="C350" t="s">
+        <v>731</v>
+      </c>
+      <c r="D350" t="s">
+        <v>13</v>
+      </c>
+      <c r="E350" t="s">
+        <v>8</v>
+      </c>
+      <c r="F350" t="s">
+        <v>576</v>
+      </c>
+      <c r="G350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A351" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B351" t="s">
+        <v>732</v>
+      </c>
+      <c r="C351" t="s">
+        <v>733</v>
+      </c>
+      <c r="D351" t="s">
+        <v>237</v>
+      </c>
+      <c r="E351" t="s">
+        <v>8</v>
+      </c>
+      <c r="F351" t="s">
+        <v>572</v>
+      </c>
+      <c r="G351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A352" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B352" t="s">
+        <v>734</v>
+      </c>
+      <c r="C352" t="s">
+        <v>735</v>
+      </c>
+      <c r="D352" t="s">
+        <v>14</v>
+      </c>
+      <c r="E352" t="s">
+        <v>8</v>
+      </c>
+      <c r="F352" t="s">
+        <v>572</v>
+      </c>
+      <c r="G352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A353" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B353" t="s">
+        <v>736</v>
+      </c>
+      <c r="C353" t="s">
+        <v>737</v>
+      </c>
+      <c r="D353" t="s">
+        <v>154</v>
+      </c>
+      <c r="E353" t="s">
+        <v>12</v>
+      </c>
+      <c r="F353" t="s">
+        <v>576</v>
+      </c>
+      <c r="G353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A354" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B354" t="s">
+        <v>738</v>
+      </c>
+      <c r="C354" t="s">
+        <v>739</v>
+      </c>
+      <c r="D354" t="s">
+        <v>16</v>
+      </c>
+      <c r="E354" t="s">
+        <v>8</v>
+      </c>
+      <c r="F354" t="s">
+        <v>572</v>
+      </c>
+      <c r="G354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A355" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B355" t="s">
+        <v>740</v>
+      </c>
+      <c r="C355" t="s">
+        <v>741</v>
+      </c>
+      <c r="D355" t="s">
+        <v>15</v>
+      </c>
+      <c r="E355" t="s">
+        <v>12</v>
+      </c>
+      <c r="F355" t="s">
+        <v>572</v>
+      </c>
+      <c r="G355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A356" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B356" t="s">
+        <v>742</v>
+      </c>
+      <c r="C356" t="s">
+        <v>743</v>
+      </c>
+      <c r="D356" t="s">
+        <v>15</v>
+      </c>
+      <c r="E356" t="s">
+        <v>12</v>
+      </c>
+      <c r="F356" t="s">
+        <v>572</v>
+      </c>
+      <c r="G356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A357" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B357" t="s">
+        <v>744</v>
+      </c>
+      <c r="C357" t="s">
+        <v>745</v>
+      </c>
+      <c r="D357" t="s">
+        <v>22</v>
+      </c>
+      <c r="E357" t="s">
+        <v>8</v>
+      </c>
+      <c r="F357" t="s">
+        <v>576</v>
+      </c>
+      <c r="G357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A358" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B358" t="s">
+        <v>746</v>
+      </c>
+      <c r="C358" t="s">
+        <v>747</v>
+      </c>
+      <c r="D358" t="s">
+        <v>11</v>
+      </c>
+      <c r="E358" t="s">
+        <v>8</v>
+      </c>
+      <c r="F358" t="s">
+        <v>572</v>
+      </c>
+      <c r="G358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A359" s="1">
+        <v>46030</v>
+      </c>
+      <c r="B359" t="s">
+        <v>748</v>
+      </c>
+      <c r="C359" t="s">
+        <v>749</v>
+      </c>
+      <c r="D359" t="s">
+        <v>116</v>
+      </c>
+      <c r="E359" t="s">
+        <v>8</v>
+      </c>
+      <c r="F359" t="s">
+        <v>571</v>
+      </c>
+      <c r="G359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A360" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B360" t="s">
+        <v>750</v>
+      </c>
+      <c r="C360" t="s">
+        <v>751</v>
+      </c>
+      <c r="D360" t="s">
+        <v>44</v>
+      </c>
+      <c r="E360" t="s">
+        <v>7</v>
+      </c>
+      <c r="F360" t="s">
+        <v>572</v>
+      </c>
+      <c r="G360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A361" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B361" t="s">
+        <v>752</v>
+      </c>
+      <c r="C361" t="s">
+        <v>753</v>
+      </c>
+      <c r="D361" t="s">
+        <v>116</v>
+      </c>
+      <c r="E361" t="s">
+        <v>8</v>
+      </c>
+      <c r="F361" t="s">
+        <v>572</v>
+      </c>
+      <c r="G361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A362" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B362" t="s">
+        <v>754</v>
+      </c>
+      <c r="C362" t="s">
+        <v>755</v>
+      </c>
+      <c r="D362" t="s">
+        <v>209</v>
+      </c>
+      <c r="E362" t="s">
+        <v>8</v>
+      </c>
+      <c r="F362" t="s">
+        <v>572</v>
+      </c>
+      <c r="G362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A363" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B363" t="s">
+        <v>756</v>
+      </c>
+      <c r="C363" t="s">
+        <v>757</v>
+      </c>
+      <c r="D363" t="s">
+        <v>134</v>
+      </c>
+      <c r="E363" t="s">
+        <v>8</v>
+      </c>
+      <c r="F363" t="s">
+        <v>572</v>
+      </c>
+      <c r="G363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A364" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B364" t="s">
+        <v>758</v>
+      </c>
+      <c r="C364" t="s">
+        <v>759</v>
+      </c>
+      <c r="D364" t="s">
+        <v>131</v>
+      </c>
+      <c r="E364" t="s">
+        <v>8</v>
+      </c>
+      <c r="F364" t="s">
+        <v>572</v>
+      </c>
+      <c r="G364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A365" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B365" t="s">
+        <v>760</v>
+      </c>
+      <c r="C365" t="s">
+        <v>761</v>
+      </c>
+      <c r="D365" t="s">
+        <v>17</v>
+      </c>
+      <c r="E365" t="s">
+        <v>8</v>
+      </c>
+      <c r="F365" t="s">
+        <v>572</v>
+      </c>
+      <c r="G365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A366" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B366" t="s">
+        <v>762</v>
+      </c>
+      <c r="C366" t="s">
+        <v>763</v>
+      </c>
+      <c r="D366" t="s">
+        <v>340</v>
+      </c>
+      <c r="E366" t="s">
+        <v>12</v>
+      </c>
+      <c r="F366" t="s">
+        <v>572</v>
+      </c>
+      <c r="G366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A367" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B367" t="s">
+        <v>764</v>
+      </c>
+      <c r="C367" t="s">
+        <v>765</v>
+      </c>
+      <c r="D367" t="s">
+        <v>6</v>
+      </c>
+      <c r="E367" t="s">
+        <v>8</v>
+      </c>
+      <c r="F367" t="s">
+        <v>572</v>
+      </c>
+      <c r="G367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A368" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B368" t="s">
+        <v>766</v>
+      </c>
+      <c r="C368" t="s">
+        <v>767</v>
+      </c>
+      <c r="D368" t="s">
+        <v>17</v>
+      </c>
+      <c r="E368" t="s">
+        <v>8</v>
+      </c>
+      <c r="F368" t="s">
+        <v>572</v>
+      </c>
+      <c r="G368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A369" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B369" t="s">
+        <v>768</v>
+      </c>
+      <c r="C369" t="s">
+        <v>769</v>
+      </c>
+      <c r="D369" t="s">
+        <v>131</v>
+      </c>
+      <c r="E369" t="s">
+        <v>8</v>
+      </c>
+      <c r="F369" t="s">
+        <v>572</v>
+      </c>
+      <c r="G369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A370" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B370" t="s">
+        <v>770</v>
+      </c>
+      <c r="C370" t="s">
+        <v>771</v>
+      </c>
+      <c r="D370" t="s">
+        <v>18</v>
+      </c>
+      <c r="E370" t="s">
+        <v>19</v>
+      </c>
+      <c r="F370" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A371" s="1">
+        <v>46031</v>
+      </c>
+      <c r="B371" t="s">
+        <v>772</v>
+      </c>
+      <c r="C371" t="s">
+        <v>773</v>
+      </c>
+      <c r="D371" t="s">
+        <v>18</v>
+      </c>
+      <c r="E371" t="s">
+        <v>19</v>
+      </c>
+      <c r="F371" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" s="1"/>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A374" s="1"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375" s="1"/>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A376" s="1"/>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A377" s="1"/>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A379" s="1"/>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A380" s="1"/>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A381" s="1"/>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A382" s="1"/>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A383" s="1"/>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A384" s="1"/>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated balde and producao - base 16/01/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-01.xlsx
+++ b/first-atlas/producao_2026-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E28BB8D-0C57-491E-A481-5BBD64460278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7189EB20-2C21-4C57-BE93-69322DF340EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
+    <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4203" uniqueCount="1724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4255" uniqueCount="1744">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -5204,10 +5204,70 @@
     <t>CONSTRUTORA SANDES SILVA LTDA</t>
   </si>
   <si>
-    <t>A procuracao precisara ser assinada digitalmente GOV.br ou procuracao publica. Em caso de assinatura digital, devera ser encaminhado o documento em formato PDF.</t>
-  </si>
-  <si>
     <t>Ata de eleicao da diretoria atualizada e registrado no orgao competente&lt;br&gt;&lt;br&gt;Estatuto social atualizado e registrado no orgao competente</t>
+  </si>
+  <si>
+    <t>13197651000165</t>
+  </si>
+  <si>
+    <t>L DE O PALLOT SERVICOS E ACABAMENTOS</t>
+  </si>
+  <si>
+    <t>19518614000198</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BEATRIZ VARELA BARROS DA SILVA</t>
+  </si>
+  <si>
+    <t>64476362000136</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LEONARDO HENRIQUE GALDINO MUNIZ</t>
+  </si>
+  <si>
+    <t>32277298000178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLAUDIA REGINA BALTAZAR CABRINI </t>
+  </si>
+  <si>
+    <t>64407841000109</t>
+  </si>
+  <si>
+    <t>L R VOIGT  LTDA</t>
+  </si>
+  <si>
+    <t>51225251000105</t>
+  </si>
+  <si>
+    <t>JTI CONSTRUTORA LTDA</t>
+  </si>
+  <si>
+    <t>17096556000126</t>
+  </si>
+  <si>
+    <t>MARCELO BISPO DE MELO COMERCIO DE COUROS</t>
+  </si>
+  <si>
+    <t>55451907000169</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ROMANCIL PEREIRA BRANCO</t>
+  </si>
+  <si>
+    <t>35158394000195</t>
+  </si>
+  <si>
+    <t>LGT CONFIA ESPORTES LTDA</t>
+  </si>
+  <si>
+    <t>16699558000228</t>
+  </si>
+  <si>
+    <t>ABIM ADMINISTRACAO DE CONDOMINIOS LTDA</t>
+  </si>
+  <si>
+    <t>Procuracao outorgada pela empresa, com poderes de representacao junto a instituicoes financeiras podendo abrir e movimentar conta corrente com mandato vigente. O solicitante da abertura de conta nao possui poderes de representacao. A procuracao precisa ser Publica, ou Digital, assinada pelo GOV. e em formato PDF.</t>
   </si>
 </sst>
 </file>
@@ -5581,9 +5641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A45A88-3D17-4433-986A-11075963C36F}">
   <dimension ref="A1:G1330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A811" workbookViewId="0">
-      <selection activeCell="B822" sqref="B822"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12955,7 +13013,7 @@
         <v>8</v>
       </c>
       <c r="F321" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G321">
         <v>0</v>
@@ -13001,7 +13059,7 @@
         <v>8</v>
       </c>
       <c r="F323" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G323">
         <v>0</v>
@@ -13300,7 +13358,7 @@
         <v>12</v>
       </c>
       <c r="F336" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G336">
         <v>0</v>
@@ -13645,7 +13703,7 @@
         <v>8</v>
       </c>
       <c r="F351" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -14217,7 +14275,7 @@
         <v>8</v>
       </c>
       <c r="F376" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="G376">
         <v>0</v>
@@ -14309,7 +14367,7 @@
         <v>12</v>
       </c>
       <c r="F380" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G380">
         <v>0</v>
@@ -14677,7 +14735,7 @@
         <v>7</v>
       </c>
       <c r="F396" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G396">
         <v>0</v>
@@ -14930,7 +14988,7 @@
         <v>8</v>
       </c>
       <c r="F407" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G407">
         <v>0</v>
@@ -16166,7 +16224,7 @@
         <v>7</v>
       </c>
       <c r="F461" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G461">
         <v>0</v>
@@ -16189,7 +16247,7 @@
         <v>7</v>
       </c>
       <c r="F462" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G462">
         <v>0</v>
@@ -16508,7 +16566,7 @@
         <v>8</v>
       </c>
       <c r="F476" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G476">
         <v>0</v>
@@ -17428,7 +17486,7 @@
         <v>12</v>
       </c>
       <c r="F516" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G516">
         <v>0</v>
@@ -17750,7 +17808,7 @@
         <v>20</v>
       </c>
       <c r="F530" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G530">
         <v>0</v>
@@ -18417,7 +18475,7 @@
         <v>12</v>
       </c>
       <c r="F559" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G559">
         <v>0</v>
@@ -18440,7 +18498,7 @@
         <v>8</v>
       </c>
       <c r="F560" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G560">
         <v>0</v>
@@ -18463,7 +18521,7 @@
         <v>7</v>
       </c>
       <c r="F561" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G561">
         <v>0</v>
@@ -18946,7 +19004,7 @@
         <v>12</v>
       </c>
       <c r="F582" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G582">
         <v>0</v>
@@ -19130,7 +19188,7 @@
         <v>8</v>
       </c>
       <c r="F590" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G590">
         <v>0</v>
@@ -19268,7 +19326,7 @@
         <v>8</v>
       </c>
       <c r="F596" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G596">
         <v>0</v>
@@ -20395,7 +20453,7 @@
         <v>12</v>
       </c>
       <c r="F645" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G645">
         <v>0</v>
@@ -20421,7 +20479,7 @@
         <v>573</v>
       </c>
       <c r="G646" t="s">
-        <v>1722</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.25">
@@ -20441,7 +20499,7 @@
         <v>8</v>
       </c>
       <c r="F647" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G647">
         <v>0</v>
@@ -20464,7 +20522,7 @@
         <v>8</v>
       </c>
       <c r="F648" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G648">
         <v>0</v>
@@ -20602,7 +20660,7 @@
         <v>12</v>
       </c>
       <c r="F654" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G654">
         <v>0</v>
@@ -20648,7 +20706,7 @@
         <v>12</v>
       </c>
       <c r="F656" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="657" spans="1:7" x14ac:dyDescent="0.25">
@@ -20898,7 +20956,7 @@
         <v>571</v>
       </c>
       <c r="G667" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="668" spans="1:7" x14ac:dyDescent="0.25">
@@ -20918,7 +20976,7 @@
         <v>7</v>
       </c>
       <c r="F668" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G668">
         <v>0</v>
@@ -20964,7 +21022,7 @@
         <v>12</v>
       </c>
       <c r="F670" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G670">
         <v>0</v>
@@ -21010,7 +21068,7 @@
         <v>7</v>
       </c>
       <c r="F672" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G672">
         <v>0</v>
@@ -21079,7 +21137,7 @@
         <v>8</v>
       </c>
       <c r="F675" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G675">
         <v>0</v>
@@ -21125,7 +21183,7 @@
         <v>7</v>
       </c>
       <c r="F677" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G677">
         <v>0</v>
@@ -21194,7 +21252,7 @@
         <v>8</v>
       </c>
       <c r="F680" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G680">
         <v>0</v>
@@ -21424,7 +21482,7 @@
         <v>7</v>
       </c>
       <c r="F690" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G690">
         <v>0</v>
@@ -21516,7 +21574,7 @@
         <v>8</v>
       </c>
       <c r="F694" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G694">
         <v>0</v>
@@ -21631,7 +21689,7 @@
         <v>8</v>
       </c>
       <c r="F699" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G699">
         <v>0</v>
@@ -21743,7 +21801,7 @@
         <v>8</v>
       </c>
       <c r="F704" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G704">
         <v>0</v>
@@ -21789,7 +21847,7 @@
         <v>8</v>
       </c>
       <c r="F706" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G706">
         <v>0</v>
@@ -21901,7 +21959,7 @@
         <v>7</v>
       </c>
       <c r="F711" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G711">
         <v>0</v>
@@ -21947,7 +22005,7 @@
         <v>7</v>
       </c>
       <c r="F713" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G713">
         <v>0</v>
@@ -21990,7 +22048,7 @@
         <v>8</v>
       </c>
       <c r="F715" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G715">
         <v>0</v>
@@ -22059,7 +22117,7 @@
         <v>12</v>
       </c>
       <c r="F718" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G718">
         <v>0</v>
@@ -22128,7 +22186,7 @@
         <v>8</v>
       </c>
       <c r="F721" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="G721">
         <v>0</v>
@@ -22266,7 +22324,7 @@
         <v>8</v>
       </c>
       <c r="F727" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G727">
         <v>0</v>
@@ -22404,7 +22462,7 @@
         <v>8</v>
       </c>
       <c r="F733" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="G733">
         <v>0</v>
@@ -22427,7 +22485,7 @@
         <v>12</v>
       </c>
       <c r="F734" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G734">
         <v>0</v>
@@ -22473,7 +22531,7 @@
         <v>12</v>
       </c>
       <c r="F736" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="737" spans="1:7" x14ac:dyDescent="0.25">
@@ -22562,7 +22620,7 @@
         <v>8</v>
       </c>
       <c r="F740" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G740">
         <v>0</v>
@@ -22700,7 +22758,10 @@
         <v>12</v>
       </c>
       <c r="F746" t="s">
-        <v>573</v>
+        <v>569</v>
+      </c>
+      <c r="G746">
+        <v>0</v>
       </c>
     </row>
     <row r="747" spans="1:7" x14ac:dyDescent="0.25">
@@ -22722,6 +22783,9 @@
       <c r="F747" t="s">
         <v>573</v>
       </c>
+      <c r="G747">
+        <v>0</v>
+      </c>
     </row>
     <row r="748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A748" s="1">
@@ -22742,6 +22806,9 @@
       <c r="F748" t="s">
         <v>569</v>
       </c>
+      <c r="G748">
+        <v>0</v>
+      </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A749" s="1">
@@ -22762,6 +22829,9 @@
       <c r="F749" t="s">
         <v>569</v>
       </c>
+      <c r="G749">
+        <v>0</v>
+      </c>
     </row>
     <row r="750" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A750" s="1">
@@ -22782,6 +22852,9 @@
       <c r="F750" t="s">
         <v>569</v>
       </c>
+      <c r="G750">
+        <v>0</v>
+      </c>
     </row>
     <row r="751" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A751" s="1">
@@ -22802,6 +22875,9 @@
       <c r="F751" t="s">
         <v>568</v>
       </c>
+      <c r="G751">
+        <v>0</v>
+      </c>
     </row>
     <row r="752" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A752" s="1">
@@ -22822,8 +22898,11 @@
       <c r="F752" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="753" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G752">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="753" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A753" s="1">
         <v>46037</v>
       </c>
@@ -22843,7 +22922,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="754" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A754" s="1">
         <v>46037</v>
       </c>
@@ -22862,8 +22941,11 @@
       <c r="F754" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="755" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G754">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="755" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A755" s="1">
         <v>46037</v>
       </c>
@@ -22882,8 +22964,11 @@
       <c r="F755" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="756" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G755">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="756" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A756" s="1">
         <v>46037</v>
       </c>
@@ -22900,10 +22985,13 @@
         <v>7</v>
       </c>
       <c r="F756" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="757" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G756">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A757" s="1">
         <v>46037</v>
       </c>
@@ -22920,10 +23008,13 @@
         <v>12</v>
       </c>
       <c r="F757" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="758" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G757">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="758" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A758" s="1">
         <v>46037</v>
       </c>
@@ -22942,8 +23033,11 @@
       <c r="F758" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="759" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G758">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="759" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A759" s="1">
         <v>46037</v>
       </c>
@@ -22962,8 +23056,11 @@
       <c r="F759" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="760" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G759">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="760" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A760" s="1">
         <v>46037</v>
       </c>
@@ -22982,8 +23079,11 @@
       <c r="F760" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="761" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G760">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="761" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A761" s="1">
         <v>46037</v>
       </c>
@@ -23002,8 +23102,11 @@
       <c r="F761" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="762" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G761">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="762" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A762" s="1">
         <v>46037</v>
       </c>
@@ -23020,10 +23123,13 @@
         <v>8</v>
       </c>
       <c r="F762" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="763" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G762">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="763" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A763" s="1">
         <v>46037</v>
       </c>
@@ -23042,8 +23148,11 @@
       <c r="F763" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="764" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G763">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A764" s="1">
         <v>46037</v>
       </c>
@@ -23062,8 +23171,11 @@
       <c r="F764" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="765" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G764">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="765" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A765" s="1">
         <v>46037</v>
       </c>
@@ -23082,8 +23194,11 @@
       <c r="F765" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="766" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G765">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="766" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A766" s="1">
         <v>46037</v>
       </c>
@@ -23100,10 +23215,13 @@
         <v>7</v>
       </c>
       <c r="F766" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="767" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G766">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="767" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A767" s="1">
         <v>46037</v>
       </c>
@@ -23122,8 +23240,11 @@
       <c r="F767" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="768" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G767">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A768" s="1">
         <v>46037</v>
       </c>
@@ -23142,8 +23263,11 @@
       <c r="F768" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="769" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G768">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="769" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A769" s="1">
         <v>46037</v>
       </c>
@@ -23160,10 +23284,13 @@
         <v>8</v>
       </c>
       <c r="F769" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="770" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G769">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="770" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A770" s="1">
         <v>46037</v>
       </c>
@@ -23180,10 +23307,13 @@
         <v>8</v>
       </c>
       <c r="F770" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="771" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G770">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A771" s="1">
         <v>46037</v>
       </c>
@@ -23202,8 +23332,11 @@
       <c r="F771" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="772" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G771">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="772" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A772" s="1">
         <v>46037</v>
       </c>
@@ -23222,8 +23355,11 @@
       <c r="F772" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="773" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G772">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="773" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A773" s="1">
         <v>46037</v>
       </c>
@@ -23240,10 +23376,13 @@
         <v>7</v>
       </c>
       <c r="F773" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="774" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G773">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="774" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A774" s="1">
         <v>46037</v>
       </c>
@@ -23262,8 +23401,11 @@
       <c r="F774" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="775" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G774">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="775" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A775" s="1">
         <v>46037</v>
       </c>
@@ -23282,8 +23424,11 @@
       <c r="F775" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="776" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G775">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="776" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A776" s="1">
         <v>46037</v>
       </c>
@@ -23300,10 +23445,13 @@
         <v>8</v>
       </c>
       <c r="F776" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="777" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G776">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="777" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A777" s="1">
         <v>46037</v>
       </c>
@@ -23320,10 +23468,13 @@
         <v>7</v>
       </c>
       <c r="F777" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="778" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G777">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="778" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A778" s="1">
         <v>46037</v>
       </c>
@@ -23340,10 +23491,13 @@
         <v>8</v>
       </c>
       <c r="F778" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="779" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G778">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="779" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A779" s="1">
         <v>46037</v>
       </c>
@@ -23360,10 +23514,13 @@
         <v>8</v>
       </c>
       <c r="F779" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="780" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G779">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="780" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A780" s="1">
         <v>46037</v>
       </c>
@@ -23380,10 +23537,13 @@
         <v>12</v>
       </c>
       <c r="F780" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="781" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G780">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="781" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A781" s="1">
         <v>46037</v>
       </c>
@@ -23402,8 +23562,11 @@
       <c r="F781" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="782" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G781">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="782" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A782" s="1">
         <v>46037</v>
       </c>
@@ -23422,8 +23585,11 @@
       <c r="F782" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="783" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G782">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="783" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A783" s="1">
         <v>46037</v>
       </c>
@@ -23442,8 +23608,11 @@
       <c r="F783" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="784" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G783">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="784" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A784" s="1">
         <v>46037</v>
       </c>
@@ -23460,10 +23629,13 @@
         <v>8</v>
       </c>
       <c r="F784" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="785" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G784">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="785" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A785" s="1">
         <v>46037</v>
       </c>
@@ -23482,8 +23654,11 @@
       <c r="F785" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="786" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G785">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="786" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A786" s="1">
         <v>46037</v>
       </c>
@@ -23502,8 +23677,11 @@
       <c r="F786" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="787" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G786">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A787" s="1">
         <v>46037</v>
       </c>
@@ -23520,10 +23698,13 @@
         <v>8</v>
       </c>
       <c r="F787" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="788" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G787">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="788" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A788" s="1">
         <v>46037</v>
       </c>
@@ -23542,8 +23723,11 @@
       <c r="F788" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="789" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G788">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A789" s="1">
         <v>46037</v>
       </c>
@@ -23560,10 +23744,13 @@
         <v>8</v>
       </c>
       <c r="F789" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="790" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G789">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="790" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A790" s="1">
         <v>46037</v>
       </c>
@@ -23582,8 +23769,11 @@
       <c r="F790" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="791" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G790">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A791" s="1">
         <v>46037</v>
       </c>
@@ -23602,8 +23792,11 @@
       <c r="F791" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="792" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G791">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A792" s="1">
         <v>46037</v>
       </c>
@@ -23620,10 +23813,13 @@
         <v>8</v>
       </c>
       <c r="F792" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="793" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G792">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="793" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A793" s="1">
         <v>46037</v>
       </c>
@@ -23642,8 +23838,11 @@
       <c r="F793" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="794" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G793">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A794" s="1">
         <v>46037</v>
       </c>
@@ -23660,10 +23859,13 @@
         <v>7</v>
       </c>
       <c r="F794" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="795" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G794">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="795" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A795" s="1">
         <v>46037</v>
       </c>
@@ -23680,10 +23882,13 @@
         <v>8</v>
       </c>
       <c r="F795" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="796" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G795">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A796" s="1">
         <v>46037</v>
       </c>
@@ -23700,10 +23905,13 @@
         <v>8</v>
       </c>
       <c r="F796" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="797" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G796">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A797" s="1">
         <v>46037</v>
       </c>
@@ -23722,8 +23930,11 @@
       <c r="F797" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="798" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G797">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="798" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A798" s="1">
         <v>46037</v>
       </c>
@@ -23740,10 +23951,13 @@
         <v>8</v>
       </c>
       <c r="F798" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="799" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G798">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="799" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A799" s="1">
         <v>46037</v>
       </c>
@@ -23762,8 +23976,11 @@
       <c r="F799" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="800" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G799">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="800" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A800" s="1">
         <v>46037</v>
       </c>
@@ -23782,8 +23999,11 @@
       <c r="F800" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="801" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G800">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="801" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A801" s="1">
         <v>46037</v>
       </c>
@@ -23802,8 +24022,11 @@
       <c r="F801" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="802" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G801">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A802" s="1">
         <v>46037</v>
       </c>
@@ -23820,10 +24043,13 @@
         <v>8</v>
       </c>
       <c r="F802" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="803" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G802">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A803" s="1">
         <v>46037</v>
       </c>
@@ -23842,8 +24068,11 @@
       <c r="F803" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="804" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G803">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="804" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A804" s="1">
         <v>46037</v>
       </c>
@@ -23862,8 +24091,11 @@
       <c r="F804" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="805" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G804">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="805" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A805" s="1">
         <v>46037</v>
       </c>
@@ -23882,8 +24114,11 @@
       <c r="F805" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="806" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G805">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A806" s="1">
         <v>46037</v>
       </c>
@@ -23902,8 +24137,11 @@
       <c r="F806" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="807" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G806">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A807" s="1">
         <v>46037</v>
       </c>
@@ -23920,10 +24158,13 @@
         <v>8</v>
       </c>
       <c r="F807" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="808" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G807">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A808" s="1">
         <v>46037</v>
       </c>
@@ -23940,10 +24181,13 @@
         <v>8</v>
       </c>
       <c r="F808" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="809" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G808">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="809" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A809" s="1">
         <v>46037</v>
       </c>
@@ -23960,10 +24204,13 @@
         <v>8</v>
       </c>
       <c r="F809" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="810" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G809">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="810" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A810" s="1">
         <v>46037</v>
       </c>
@@ -23982,8 +24229,11 @@
       <c r="F810" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="811" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G810">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="811" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A811" s="1">
         <v>46037</v>
       </c>
@@ -24002,8 +24252,11 @@
       <c r="F811" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="812" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G811">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="812" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A812" s="1">
         <v>46037</v>
       </c>
@@ -24020,10 +24273,13 @@
         <v>8</v>
       </c>
       <c r="F812" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="813" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+      <c r="G812" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="813" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A813" s="1">
         <v>46037</v>
       </c>
@@ -24042,8 +24298,11 @@
       <c r="F813" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="814" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G813">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="814" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A814" s="1">
         <v>46037</v>
       </c>
@@ -24062,8 +24321,11 @@
       <c r="F814" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="815" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G814">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="815" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A815" s="1">
         <v>46037</v>
       </c>
@@ -24082,8 +24344,11 @@
       <c r="F815" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="816" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G815">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="816" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A816" s="1">
         <v>46037</v>
       </c>
@@ -24102,8 +24367,11 @@
       <c r="F816" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="817" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G816">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="817" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A817" s="1">
         <v>46037</v>
       </c>
@@ -24122,8 +24390,11 @@
       <c r="F817" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="818" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G817">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="818" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A818" s="1">
         <v>46037</v>
       </c>
@@ -24142,8 +24413,11 @@
       <c r="F818" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="819" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G818">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="819" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A819" s="1">
         <v>46037</v>
       </c>
@@ -24160,10 +24434,13 @@
         <v>8</v>
       </c>
       <c r="F819" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="820" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G819">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="820" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A820" s="1">
         <v>46037</v>
       </c>
@@ -24182,8 +24459,11 @@
       <c r="F820" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="821" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G820">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="821" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A821" s="1">
         <v>46037</v>
       </c>
@@ -24200,10 +24480,13 @@
         <v>8</v>
       </c>
       <c r="F821" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="822" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G821">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="822" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A822" s="1">
         <v>46037</v>
       </c>
@@ -24220,10 +24503,13 @@
         <v>7</v>
       </c>
       <c r="F822" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="823" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G822">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="823" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A823" s="1">
         <v>46037</v>
       </c>
@@ -24242,8 +24528,11 @@
       <c r="F823" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="824" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G823">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="824" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A824" s="1">
         <v>46037</v>
       </c>
@@ -24262,8 +24551,11 @@
       <c r="F824" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="825" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G824">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="825" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A825" s="1">
         <v>46037</v>
       </c>
@@ -24282,8 +24574,11 @@
       <c r="F825" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="826" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G825">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="826" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A826" s="1">
         <v>46037</v>
       </c>
@@ -24302,8 +24597,11 @@
       <c r="F826" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="827" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G826">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="827" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A827" s="1">
         <v>46037</v>
       </c>
@@ -24322,8 +24620,11 @@
       <c r="F827" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="828" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G827">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="828" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A828" s="1">
         <v>46037</v>
       </c>
@@ -24340,10 +24641,13 @@
         <v>7</v>
       </c>
       <c r="F828" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="829" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+      <c r="G828" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="829" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A829" s="1">
         <v>46037</v>
       </c>
@@ -24360,10 +24664,13 @@
         <v>8</v>
       </c>
       <c r="F829" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="830" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G829">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="830" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A830" s="1">
         <v>46037</v>
       </c>
@@ -24380,10 +24687,13 @@
         <v>8</v>
       </c>
       <c r="F830" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="831" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G830">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="831" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A831" s="1">
         <v>46037</v>
       </c>
@@ -24402,8 +24712,11 @@
       <c r="F831" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="832" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G831">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="832" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A832" s="1">
         <v>46037</v>
       </c>
@@ -24422,8 +24735,11 @@
       <c r="F832" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="833" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G832">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="833" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A833" s="1">
         <v>46037</v>
       </c>
@@ -24442,8 +24758,11 @@
       <c r="F833" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="834" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G833">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="834" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A834" s="1">
         <v>46037</v>
       </c>
@@ -24462,8 +24781,11 @@
       <c r="F834" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="835" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G834">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="835" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A835" s="1">
         <v>46037</v>
       </c>
@@ -24480,10 +24802,13 @@
         <v>8</v>
       </c>
       <c r="F835" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="836" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G835">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="836" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A836" s="1">
         <v>46037</v>
       </c>
@@ -24500,10 +24825,13 @@
         <v>8</v>
       </c>
       <c r="F836" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="837" spans="1:6" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="G836">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="837" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A837" s="1">
         <v>46037</v>
       </c>
@@ -24520,10 +24848,13 @@
         <v>8</v>
       </c>
       <c r="F837" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="838" spans="1:6" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="G837">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="838" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A838" s="1">
         <v>46037</v>
       </c>
@@ -24540,38 +24871,241 @@
         <v>7</v>
       </c>
       <c r="F838" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="839" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A839" s="1"/>
-    </row>
-    <row r="840" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A840" s="1"/>
-    </row>
-    <row r="841" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A841" s="1"/>
-    </row>
-    <row r="842" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A842" s="1"/>
-    </row>
-    <row r="843" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A843" s="1"/>
-    </row>
-    <row r="844" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A844" s="1"/>
-    </row>
-    <row r="845" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A845" s="1"/>
-    </row>
-    <row r="846" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A846" s="1"/>
-    </row>
-    <row r="847" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A847" s="1"/>
-    </row>
-    <row r="848" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A848" s="1"/>
+        <v>569</v>
+      </c>
+      <c r="G838">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="839" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A839" s="1">
+        <v>46037</v>
+      </c>
+      <c r="B839" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C839" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D839" t="s">
+        <v>16</v>
+      </c>
+      <c r="E839" t="s">
+        <v>8</v>
+      </c>
+      <c r="F839" t="s">
+        <v>569</v>
+      </c>
+      <c r="G839">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="840" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A840" s="1">
+        <v>46037</v>
+      </c>
+      <c r="B840" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C840" t="s">
+        <v>1726</v>
+      </c>
+      <c r="D840" t="s">
+        <v>16</v>
+      </c>
+      <c r="E840" t="s">
+        <v>8</v>
+      </c>
+      <c r="F840" t="s">
+        <v>569</v>
+      </c>
+      <c r="G840">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="841" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A841" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B841" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C841" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D841" t="s">
+        <v>116</v>
+      </c>
+      <c r="E841" t="s">
+        <v>8</v>
+      </c>
+      <c r="F841" t="s">
+        <v>569</v>
+      </c>
+      <c r="G841">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="842" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A842" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B842" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C842" t="s">
+        <v>1730</v>
+      </c>
+      <c r="D842" t="s">
+        <v>134</v>
+      </c>
+      <c r="E842" t="s">
+        <v>8</v>
+      </c>
+      <c r="F842" t="s">
+        <v>569</v>
+      </c>
+      <c r="G842">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="843" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A843" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B843" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C843" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D843" t="s">
+        <v>23</v>
+      </c>
+      <c r="E843" t="s">
+        <v>8</v>
+      </c>
+      <c r="F843" t="s">
+        <v>569</v>
+      </c>
+      <c r="G843">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="844" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A844" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B844" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C844" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D844" t="s">
+        <v>9</v>
+      </c>
+      <c r="E844" t="s">
+        <v>8</v>
+      </c>
+      <c r="F844" t="s">
+        <v>569</v>
+      </c>
+      <c r="G844">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="845" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A845" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B845" t="s">
+        <v>1735</v>
+      </c>
+      <c r="C845" t="s">
+        <v>1736</v>
+      </c>
+      <c r="D845" t="s">
+        <v>116</v>
+      </c>
+      <c r="E845" t="s">
+        <v>8</v>
+      </c>
+      <c r="F845" t="s">
+        <v>569</v>
+      </c>
+      <c r="G845">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="846" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A846" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B846" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C846" t="s">
+        <v>1738</v>
+      </c>
+      <c r="D846" t="s">
+        <v>134</v>
+      </c>
+      <c r="E846" t="s">
+        <v>8</v>
+      </c>
+      <c r="F846" t="s">
+        <v>569</v>
+      </c>
+      <c r="G846">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="847" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A847" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B847" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C847" t="s">
+        <v>1740</v>
+      </c>
+      <c r="D847" t="s">
+        <v>44</v>
+      </c>
+      <c r="E847" t="s">
+        <v>7</v>
+      </c>
+      <c r="F847" t="s">
+        <v>569</v>
+      </c>
+      <c r="G847">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="848" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A848" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B848" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C848" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D848" t="s">
+        <v>11</v>
+      </c>
+      <c r="E848" t="s">
+        <v>8</v>
+      </c>
+      <c r="F848" t="s">
+        <v>569</v>
+      </c>
+      <c r="G848">
+        <v>0</v>
+      </c>
     </row>
     <row r="849" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A849" s="1"/>

</xml_diff>

<commit_message>
updated balde and producao - base 19/01/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-01.xlsx
+++ b/first-atlas/producao_2026-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7189EB20-2C21-4C57-BE93-69322DF340EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B3A7EF-6174-4B20-AC55-675942D0EE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4255" uniqueCount="1744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4701" uniqueCount="1924">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -5268,6 +5268,546 @@
   </si>
   <si>
     <t>Procuracao outorgada pela empresa, com poderes de representacao junto a instituicoes financeiras podendo abrir e movimentar conta corrente com mandato vigente. O solicitante da abertura de conta nao possui poderes de representacao. A procuracao precisa ser Publica, ou Digital, assinada pelo GOV. e em formato PDF.</t>
+  </si>
+  <si>
+    <t>63127681000173</t>
+  </si>
+  <si>
+    <t>SAMUEL MATHEUS APARECIDO FENERICH</t>
+  </si>
+  <si>
+    <t>58818811000265</t>
+  </si>
+  <si>
+    <t>KC BATERIAS LTDA</t>
+  </si>
+  <si>
+    <t>64200015000186</t>
+  </si>
+  <si>
+    <t>CARVALHO PSICOLOGIA APLICADA LTDA</t>
+  </si>
+  <si>
+    <t>60695215000104</t>
+  </si>
+  <si>
+    <t>AGROPECUARIA FAZENDA SAO JOSE LTDA</t>
+  </si>
+  <si>
+    <t>40834366000180</t>
+  </si>
+  <si>
+    <t>CONSULTORIO ODONTOLOGICO DR. JOSSIVAN CAMPOS LTDA</t>
+  </si>
+  <si>
+    <t>28074369000168</t>
+  </si>
+  <si>
+    <t>DANIEL OSEIAS DE PAULA</t>
+  </si>
+  <si>
+    <t>64409836000127</t>
+  </si>
+  <si>
+    <t>JPMN COMERCIO DE ELETRICOS E HIDRAULICOS LTDA</t>
+  </si>
+  <si>
+    <t>64451603000192</t>
+  </si>
+  <si>
+    <t>F L MATIAS SERVICOS</t>
+  </si>
+  <si>
+    <t>64077881000121</t>
+  </si>
+  <si>
+    <t>JOAO VICTOR ALMEIDA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>64375617000174</t>
+  </si>
+  <si>
+    <t>FABIANO LUIZ CERQUEIRA DA CONCEICAO</t>
+  </si>
+  <si>
+    <t>59771230000105</t>
+  </si>
+  <si>
+    <t>GURIU COMERCIO DA MATERIAL DE CONSTRUCAO LTDA</t>
+  </si>
+  <si>
+    <t>64504272000101</t>
+  </si>
+  <si>
+    <t>IADA AVIATION LTDA</t>
+  </si>
+  <si>
+    <t>60169282000187</t>
+  </si>
+  <si>
+    <t>BAG MANIA LTDA</t>
+  </si>
+  <si>
+    <t>58433309000155</t>
+  </si>
+  <si>
+    <t>DEBORA CRISTIANE FERREIRA JACOBUCCI SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>64493642000152</t>
+  </si>
+  <si>
+    <t>M V CORDEIRO MARQUES COMERCIO</t>
+  </si>
+  <si>
+    <t>64505057000125</t>
+  </si>
+  <si>
+    <t>JSL PRESTADORA DE SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>10443222000132</t>
+  </si>
+  <si>
+    <t>MARCOS AIR RAMOS BRITO</t>
+  </si>
+  <si>
+    <t>56115216000157</t>
+  </si>
+  <si>
+    <t>LAGOINHA FROTAS LTDA</t>
+  </si>
+  <si>
+    <t>64496246000189</t>
+  </si>
+  <si>
+    <t>FENIX STUDIO DE DANCA LTDA</t>
+  </si>
+  <si>
+    <t>39504908000178</t>
+  </si>
+  <si>
+    <t>FERNANDO ALENCAR DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>62607447000180</t>
+  </si>
+  <si>
+    <t>ESSENTIS SAUDE LTDA</t>
+  </si>
+  <si>
+    <t>36534397000220</t>
+  </si>
+  <si>
+    <t>R.F. CARDOSO HASHTAG TURISMO LTDA</t>
+  </si>
+  <si>
+    <t>64509519000182</t>
+  </si>
+  <si>
+    <t>R M CARRENHO</t>
+  </si>
+  <si>
+    <t>61921205000102</t>
+  </si>
+  <si>
+    <t>GOOD SEED ASSESSORIA E CONSULTORIA LTDA</t>
+  </si>
+  <si>
+    <t>58638259000142</t>
+  </si>
+  <si>
+    <t>DEPOSITO DE BEBIDAS DOIS IRMAOS ARANGO LTDA</t>
+  </si>
+  <si>
+    <t>32172485000197</t>
+  </si>
+  <si>
+    <t>MRC7 EXPERIENCE LTDA</t>
+  </si>
+  <si>
+    <t>64503181000151</t>
+  </si>
+  <si>
+    <t>EJC MORAES VEICULOS LTDA</t>
+  </si>
+  <si>
+    <t>58845222000195</t>
+  </si>
+  <si>
+    <t>F PADILHA TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>05087068000173</t>
+  </si>
+  <si>
+    <t>G.T.C.DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>39802251000125</t>
+  </si>
+  <si>
+    <t>PEDROSO COMERCIAL DE CARNE LTDA</t>
+  </si>
+  <si>
+    <t>04327549000146</t>
+  </si>
+  <si>
+    <t>CIR - CONEXOES DE REDES LTDA</t>
+  </si>
+  <si>
+    <t>40131281000136</t>
+  </si>
+  <si>
+    <t>NUTRICIONISTA FLAVIA ROQUE LTDA</t>
+  </si>
+  <si>
+    <t>14639339000147</t>
+  </si>
+  <si>
+    <t>3IN INTERMEDIACOES E SOLUCOES EMPRESARIAIS LTDA</t>
+  </si>
+  <si>
+    <t>64476090000174</t>
+  </si>
+  <si>
+    <t>CAMARGOS BATISTA CORRETORA DE SEGUROS LTDA</t>
+  </si>
+  <si>
+    <t>15769083000155</t>
+  </si>
+  <si>
+    <t>DW CARGO EXPRESS LTDA</t>
+  </si>
+  <si>
+    <t>50859371000100</t>
+  </si>
+  <si>
+    <t>EMPORIO E LANCHONETE PREMIUM LTDA</t>
+  </si>
+  <si>
+    <t>64466356000106</t>
+  </si>
+  <si>
+    <t>ELETRONICA LIMA LTDA</t>
+  </si>
+  <si>
+    <t>60435728000178</t>
+  </si>
+  <si>
+    <t>LBN SOROCABA TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>64484670000103</t>
+  </si>
+  <si>
+    <t>SANDZ ECOM LTDA</t>
+  </si>
+  <si>
+    <t>Joao Pedro Gabriel Troiano</t>
+  </si>
+  <si>
+    <t>34925757000108</t>
+  </si>
+  <si>
+    <t>34.925.757 ISMAEL SERAFIM DA SILVA</t>
+  </si>
+  <si>
+    <t>20822208000101</t>
+  </si>
+  <si>
+    <t>TURISMO ALTO DA SERRA E ADEGA PANATO LTDA</t>
+  </si>
+  <si>
+    <t>60140627000170</t>
+  </si>
+  <si>
+    <t>GUILHERME FRAZAO REPRESENTACOES COMERCIAIS</t>
+  </si>
+  <si>
+    <t>57058797000103</t>
+  </si>
+  <si>
+    <t>RICARDO SIMPLICIO DA SILVA</t>
+  </si>
+  <si>
+    <t>60035600000117</t>
+  </si>
+  <si>
+    <t>CENTRO TERAPEUTICO CT DECIDIR LTDA</t>
+  </si>
+  <si>
+    <t>17888044000100</t>
+  </si>
+  <si>
+    <t>LUIZ FERNANDO PEREIRA ARRUDA</t>
+  </si>
+  <si>
+    <t>19020959000117</t>
+  </si>
+  <si>
+    <t>ALEX S. DIAS DE SOUZA SERRALHERIA</t>
+  </si>
+  <si>
+    <t>38113210000169</t>
+  </si>
+  <si>
+    <t>KATYUZA MARQUES FARIA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>37107124000180</t>
+  </si>
+  <si>
+    <t>BRUNO WALBERTO DE JESUS ANDRADE</t>
+  </si>
+  <si>
+    <t>42678545000100</t>
+  </si>
+  <si>
+    <t>PARAOPEBA FUTEBOL CLUBE</t>
+  </si>
+  <si>
+    <t>35950826000104</t>
+  </si>
+  <si>
+    <t>MR TENIS ESCOLA DE ESPORTE LTDA</t>
+  </si>
+  <si>
+    <t>41599773000113</t>
+  </si>
+  <si>
+    <t>LAIANY VILA BIZARO COLETA DE RESIDUOS LTDA</t>
+  </si>
+  <si>
+    <t>49412391000140</t>
+  </si>
+  <si>
+    <t>TRACKER BRASIL MONITORAMENTO VEICULAR LTDA</t>
+  </si>
+  <si>
+    <t>64475014000144</t>
+  </si>
+  <si>
+    <t>IPANEMA SERVICOS DE CUIDADOS DE PESSOAS LTDA.</t>
+  </si>
+  <si>
+    <t>24455063000109</t>
+  </si>
+  <si>
+    <t>M&amp;M CONSTRUCOES E INCORPORACOES LTDA</t>
+  </si>
+  <si>
+    <t>00319659000105</t>
+  </si>
+  <si>
+    <t>ANTOLOGICA CONSULTORIA EDICOES E EVENTOS LTDA</t>
+  </si>
+  <si>
+    <t>64328160000147</t>
+  </si>
+  <si>
+    <t>Rebeca Moda Jeans</t>
+  </si>
+  <si>
+    <t>61172906000188</t>
+  </si>
+  <si>
+    <t>JOCA PISOS E REVESTIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>61629638000180</t>
+  </si>
+  <si>
+    <t>E. MARTINS DAS CHAGAS</t>
+  </si>
+  <si>
+    <t>64309929000180</t>
+  </si>
+  <si>
+    <t>ISMAEL SOUSA DE ARAUJO</t>
+  </si>
+  <si>
+    <t>64327764000179</t>
+  </si>
+  <si>
+    <t>INSPRO INSPECAO VEICULAR LTDA</t>
+  </si>
+  <si>
+    <t>45232308000109</t>
+  </si>
+  <si>
+    <t>UP ONE TURISMO LTDA</t>
+  </si>
+  <si>
+    <t>64220222000100</t>
+  </si>
+  <si>
+    <t>PALHETA EXCELENTE PARTICIPACOES LTDA</t>
+  </si>
+  <si>
+    <t>64445260000153</t>
+  </si>
+  <si>
+    <t>CAFETERIA CAVALO BRANCO LTDA</t>
+  </si>
+  <si>
+    <t>51167688000130</t>
+  </si>
+  <si>
+    <t>N S V TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>36764831000187</t>
+  </si>
+  <si>
+    <t>CASPON SERVICOS TERCEIRIZADOS LTDA</t>
+  </si>
+  <si>
+    <t>62461076000171</t>
+  </si>
+  <si>
+    <t>MF NOGUEIRA REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>37719487000177</t>
+  </si>
+  <si>
+    <t>MARCONI CUTRIM COSTA</t>
+  </si>
+  <si>
+    <t>17747633000160</t>
+  </si>
+  <si>
+    <t>RAISSA TEIXEIRA PIMENTEL DE SOUSA</t>
+  </si>
+  <si>
+    <t>53962244000111</t>
+  </si>
+  <si>
+    <t>VIDRACEIRO CAMARGO LTDA</t>
+  </si>
+  <si>
+    <t>50156935000130</t>
+  </si>
+  <si>
+    <t>REPRESENTACOES CRB LTDA</t>
+  </si>
+  <si>
+    <t>54195740000150</t>
+  </si>
+  <si>
+    <t>LUIZ PHELIPE MELO DO ESPIRITO SANTO</t>
+  </si>
+  <si>
+    <t>64270976000167</t>
+  </si>
+  <si>
+    <t>BENEVENTO PRESTACIONAL LTDA</t>
+  </si>
+  <si>
+    <t>63969551000188</t>
+  </si>
+  <si>
+    <t>LVM CONSULTORIA E REPRESENTACAO COMERCIAL LTDA</t>
+  </si>
+  <si>
+    <t>Felipe Silva</t>
+  </si>
+  <si>
+    <t>52552560000152</t>
+  </si>
+  <si>
+    <t>LUCIANO RODRIGO APARICIO PRAXEDES</t>
+  </si>
+  <si>
+    <t>32467280000139</t>
+  </si>
+  <si>
+    <t>MARINA SOARES DE CARVALHO</t>
+  </si>
+  <si>
+    <t>64226235000189</t>
+  </si>
+  <si>
+    <t>WR CONTABILIDADE E CONSULTORIA EMPRESARIAL LTDA</t>
+  </si>
+  <si>
+    <t>13172332000103</t>
+  </si>
+  <si>
+    <t>R S GUIMARAES LTDA</t>
+  </si>
+  <si>
+    <t>28399545000131</t>
+  </si>
+  <si>
+    <t>28.399.545 AUGUSTO CEZAR NASCIMENTO DE MENDONCA</t>
+  </si>
+  <si>
+    <t>54414129000175</t>
+  </si>
+  <si>
+    <t>ADEQUA - ENGENHARIA E SOLUCOES PARA CONSTRUCAO LTDA</t>
+  </si>
+  <si>
+    <t>61995241000102</t>
+  </si>
+  <si>
+    <t>A. PAULINO PEDRO PINTURA LTDA</t>
+  </si>
+  <si>
+    <t>41886503000193</t>
+  </si>
+  <si>
+    <t>MAX POINT BAR E CHOPERIA LTDA</t>
+  </si>
+  <si>
+    <t>37865804000163</t>
+  </si>
+  <si>
+    <t>EAGLE VISION LTDA</t>
+  </si>
+  <si>
+    <t>19420780000157</t>
+  </si>
+  <si>
+    <t>JAVA HOUSE PASTELARIA LTDA</t>
+  </si>
+  <si>
+    <t>63894134000113</t>
+  </si>
+  <si>
+    <t>TC SOLUCOES INDUSTRIAIS LTDA</t>
+  </si>
+  <si>
+    <t>37780218000116</t>
+  </si>
+  <si>
+    <t>EMPREITEIRA FORNAZIERO LTDA</t>
+  </si>
+  <si>
+    <t>26608060000185</t>
+  </si>
+  <si>
+    <t>NILTON CESAR DOS SANTOS SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>43637573000133</t>
+  </si>
+  <si>
+    <t>EVANDRO ALVES SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>64437865000100</t>
+  </si>
+  <si>
+    <t>MARMORARIA EVOLUCAO LTDA</t>
+  </si>
+  <si>
+    <t>17904348000106</t>
+  </si>
+  <si>
+    <t>SSJ CASTRO DECORACOES E INTERIORES LTDA</t>
   </si>
 </sst>
 </file>
@@ -5641,7 +6181,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A45A88-3D17-4433-986A-11075963C36F}">
   <dimension ref="A1:G1330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A918" workbookViewId="0">
+      <selection activeCell="F937" sqref="F937"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14804,7 +15346,7 @@
         <v>8</v>
       </c>
       <c r="F399" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="G399">
         <v>0</v>
@@ -22962,7 +23504,7 @@
         <v>8</v>
       </c>
       <c r="F755" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G755">
         <v>0</v>
@@ -23261,7 +23803,7 @@
         <v>8</v>
       </c>
       <c r="F768" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G768">
         <v>0</v>
@@ -23767,7 +24309,7 @@
         <v>7</v>
       </c>
       <c r="F790" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G790">
         <v>0</v>
@@ -24112,7 +24654,7 @@
         <v>8</v>
       </c>
       <c r="F805" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G805">
         <v>0</v>
@@ -24135,7 +24677,7 @@
         <v>8</v>
       </c>
       <c r="F806" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G806">
         <v>0</v>
@@ -24641,7 +25183,7 @@
         <v>7</v>
       </c>
       <c r="F828" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="G828" t="s">
         <v>1161</v>
@@ -24756,7 +25298,7 @@
         <v>7</v>
       </c>
       <c r="F833" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="G833">
         <v>0</v>
@@ -25107,292 +25649,2069 @@
         <v>0</v>
       </c>
     </row>
-    <row r="849" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A849" s="1"/>
-    </row>
-    <row r="850" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A850" s="1"/>
-    </row>
-    <row r="851" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A851" s="1"/>
-    </row>
-    <row r="852" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A852" s="1"/>
-    </row>
-    <row r="853" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A853" s="1"/>
-    </row>
-    <row r="854" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A854" s="1"/>
-    </row>
-    <row r="855" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A855" s="1"/>
-    </row>
-    <row r="856" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A856" s="1"/>
-    </row>
-    <row r="857" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A857" s="1"/>
-    </row>
-    <row r="858" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A858" s="1"/>
-    </row>
-    <row r="859" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A859" s="1"/>
-    </row>
-    <row r="860" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A860" s="1"/>
-    </row>
-    <row r="861" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A861" s="1"/>
-    </row>
-    <row r="862" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A862" s="1"/>
-    </row>
-    <row r="863" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A863" s="1"/>
-    </row>
-    <row r="864" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A864" s="1"/>
-    </row>
-    <row r="865" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A865" s="1"/>
-    </row>
-    <row r="866" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A866" s="1"/>
-    </row>
-    <row r="867" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A867" s="1"/>
-    </row>
-    <row r="868" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A868" s="1"/>
-    </row>
-    <row r="869" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A869" s="1"/>
-    </row>
-    <row r="870" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A870" s="1"/>
-    </row>
-    <row r="871" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A871" s="1"/>
-    </row>
-    <row r="872" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A872" s="1"/>
-    </row>
-    <row r="873" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A873" s="1"/>
-    </row>
-    <row r="874" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A874" s="1"/>
-    </row>
-    <row r="875" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A875" s="1"/>
-    </row>
-    <row r="876" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A876" s="1"/>
-    </row>
-    <row r="877" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A877" s="1"/>
-    </row>
-    <row r="878" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A878" s="1"/>
-    </row>
-    <row r="879" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A879" s="1"/>
-    </row>
-    <row r="880" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A880" s="1"/>
-    </row>
-    <row r="881" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A881" s="1"/>
-    </row>
-    <row r="882" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A882" s="1"/>
-    </row>
-    <row r="883" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A883" s="1"/>
-    </row>
-    <row r="884" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A884" s="1"/>
-    </row>
-    <row r="885" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A885" s="1"/>
-    </row>
-    <row r="886" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A886" s="1"/>
-    </row>
-    <row r="887" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A887" s="1"/>
-    </row>
-    <row r="888" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A888" s="1"/>
-    </row>
-    <row r="889" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A889" s="1"/>
-    </row>
-    <row r="890" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A890" s="1"/>
-    </row>
-    <row r="891" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A891" s="1"/>
-    </row>
-    <row r="892" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A892" s="1"/>
-    </row>
-    <row r="893" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A893" s="1"/>
-    </row>
-    <row r="894" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A894" s="1"/>
-    </row>
-    <row r="895" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A895" s="1"/>
-    </row>
-    <row r="896" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A896" s="1"/>
-    </row>
-    <row r="897" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A897" s="1"/>
-    </row>
-    <row r="898" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A898" s="1"/>
-    </row>
-    <row r="899" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A899" s="1"/>
-    </row>
-    <row r="900" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A900" s="1"/>
-    </row>
-    <row r="901" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A901" s="1"/>
-    </row>
-    <row r="902" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A902" s="1"/>
-    </row>
-    <row r="903" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A903" s="1"/>
-    </row>
-    <row r="904" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A904" s="1"/>
-    </row>
-    <row r="905" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A905" s="1"/>
-    </row>
-    <row r="906" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A906" s="1"/>
-    </row>
-    <row r="907" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A907" s="1"/>
-    </row>
-    <row r="908" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A908" s="1"/>
-    </row>
-    <row r="909" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A909" s="1"/>
-    </row>
-    <row r="910" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A910" s="1"/>
-    </row>
-    <row r="911" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A911" s="1"/>
-    </row>
-    <row r="912" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A912" s="1"/>
-    </row>
-    <row r="913" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A913" s="1"/>
-    </row>
-    <row r="914" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A914" s="1"/>
-    </row>
-    <row r="915" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A915" s="1"/>
-    </row>
-    <row r="916" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A916" s="1"/>
-    </row>
-    <row r="917" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A917" s="1"/>
-    </row>
-    <row r="918" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A918" s="1"/>
-    </row>
-    <row r="919" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A919" s="1"/>
-    </row>
-    <row r="920" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A920" s="1"/>
-    </row>
-    <row r="921" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A921" s="1"/>
-    </row>
-    <row r="922" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A922" s="1"/>
-    </row>
-    <row r="923" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A923" s="1"/>
-    </row>
-    <row r="924" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A924" s="1"/>
-    </row>
-    <row r="925" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A925" s="1"/>
-    </row>
-    <row r="926" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A926" s="1"/>
-    </row>
-    <row r="927" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A927" s="1"/>
-    </row>
-    <row r="928" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A928" s="1"/>
-    </row>
-    <row r="929" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A929" s="1"/>
-    </row>
-    <row r="930" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A930" s="1"/>
-    </row>
-    <row r="931" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A931" s="1"/>
-    </row>
-    <row r="932" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A932" s="1"/>
-    </row>
-    <row r="933" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A933" s="1"/>
-    </row>
-    <row r="934" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A934" s="1"/>
-    </row>
-    <row r="935" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A935" s="1"/>
-    </row>
-    <row r="936" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A936" s="1"/>
-    </row>
-    <row r="937" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A937" s="1"/>
-    </row>
-    <row r="938" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A849" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B849" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C849" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D849" t="s">
+        <v>18</v>
+      </c>
+      <c r="E849" t="s">
+        <v>19</v>
+      </c>
+      <c r="F849" t="s">
+        <v>569</v>
+      </c>
+      <c r="G849">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="850" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A850" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B850" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C850" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D850" t="s">
+        <v>10</v>
+      </c>
+      <c r="E850" t="s">
+        <v>8</v>
+      </c>
+      <c r="F850" t="s">
+        <v>569</v>
+      </c>
+      <c r="G850">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="851" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A851" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B851" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C851" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D851" t="s">
+        <v>14</v>
+      </c>
+      <c r="E851" t="s">
+        <v>8</v>
+      </c>
+      <c r="F851" t="s">
+        <v>569</v>
+      </c>
+      <c r="G851">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="852" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A852" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B852" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C852" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D852" t="s">
+        <v>16</v>
+      </c>
+      <c r="E852" t="s">
+        <v>8</v>
+      </c>
+      <c r="F852" t="s">
+        <v>569</v>
+      </c>
+      <c r="G852">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="853" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A853" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B853" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C853" t="s">
+        <v>1753</v>
+      </c>
+      <c r="D853" t="s">
+        <v>17</v>
+      </c>
+      <c r="E853" t="s">
+        <v>8</v>
+      </c>
+      <c r="F853" t="s">
+        <v>569</v>
+      </c>
+      <c r="G853">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="854" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A854" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B854" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C854" t="s">
+        <v>1755</v>
+      </c>
+      <c r="D854" t="s">
+        <v>22</v>
+      </c>
+      <c r="E854" t="s">
+        <v>7</v>
+      </c>
+      <c r="F854" t="s">
+        <v>569</v>
+      </c>
+      <c r="G854">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="855" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A855" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B855" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C855" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D855" t="s">
+        <v>209</v>
+      </c>
+      <c r="E855" t="s">
+        <v>12</v>
+      </c>
+      <c r="F855" t="s">
+        <v>569</v>
+      </c>
+      <c r="G855">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="856" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A856" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B856" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C856" t="s">
+        <v>1759</v>
+      </c>
+      <c r="D856" t="s">
+        <v>237</v>
+      </c>
+      <c r="E856" t="s">
+        <v>12</v>
+      </c>
+      <c r="F856" t="s">
+        <v>569</v>
+      </c>
+      <c r="G856">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="857" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A857" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B857" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C857" t="s">
+        <v>1761</v>
+      </c>
+      <c r="D857" t="s">
+        <v>14</v>
+      </c>
+      <c r="E857" t="s">
+        <v>8</v>
+      </c>
+      <c r="F857" t="s">
+        <v>569</v>
+      </c>
+      <c r="G857">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="858" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A858" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B858" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C858" t="s">
+        <v>1763</v>
+      </c>
+      <c r="D858" t="s">
+        <v>113</v>
+      </c>
+      <c r="E858" t="s">
+        <v>7</v>
+      </c>
+      <c r="F858" t="s">
+        <v>569</v>
+      </c>
+      <c r="G858">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="859" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A859" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B859" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C859" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D859" t="s">
+        <v>6</v>
+      </c>
+      <c r="E859" t="s">
+        <v>8</v>
+      </c>
+      <c r="F859" t="s">
+        <v>569</v>
+      </c>
+      <c r="G859">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="860" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A860" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B860" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C860" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D860" t="s">
+        <v>113</v>
+      </c>
+      <c r="E860" t="s">
+        <v>7</v>
+      </c>
+      <c r="F860" t="s">
+        <v>573</v>
+      </c>
+      <c r="G860">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="861" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A861" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B861" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C861" t="s">
+        <v>1769</v>
+      </c>
+      <c r="D861" t="s">
+        <v>11</v>
+      </c>
+      <c r="E861" t="s">
+        <v>8</v>
+      </c>
+      <c r="F861" t="s">
+        <v>569</v>
+      </c>
+      <c r="G861">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="862" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A862" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B862" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C862" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D862" t="s">
+        <v>17</v>
+      </c>
+      <c r="E862" t="s">
+        <v>8</v>
+      </c>
+      <c r="F862" t="s">
+        <v>569</v>
+      </c>
+      <c r="G862">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="863" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A863" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B863" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C863" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D863" t="s">
+        <v>154</v>
+      </c>
+      <c r="E863" t="s">
+        <v>12</v>
+      </c>
+      <c r="F863" t="s">
+        <v>569</v>
+      </c>
+      <c r="G863">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="864" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A864" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B864" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C864" t="s">
+        <v>1775</v>
+      </c>
+      <c r="D864" t="s">
+        <v>209</v>
+      </c>
+      <c r="E864" t="s">
+        <v>12</v>
+      </c>
+      <c r="F864" t="s">
+        <v>570</v>
+      </c>
+      <c r="G864">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="865" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A865" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B865" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C865" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D865" t="s">
+        <v>116</v>
+      </c>
+      <c r="E865" t="s">
+        <v>8</v>
+      </c>
+      <c r="F865" t="s">
+        <v>570</v>
+      </c>
+      <c r="G865">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="866" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A866" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B866" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C866" t="s">
+        <v>1779</v>
+      </c>
+      <c r="D866" t="s">
+        <v>22</v>
+      </c>
+      <c r="E866" t="s">
+        <v>7</v>
+      </c>
+      <c r="F866" t="s">
+        <v>569</v>
+      </c>
+      <c r="G866">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="867" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A867" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B867" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C867" t="s">
+        <v>1781</v>
+      </c>
+      <c r="D867" t="s">
+        <v>154</v>
+      </c>
+      <c r="E867" t="s">
+        <v>12</v>
+      </c>
+      <c r="F867" t="s">
+        <v>573</v>
+      </c>
+      <c r="G867">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="868" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A868" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B868" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C868" t="s">
+        <v>1783</v>
+      </c>
+      <c r="D868" t="s">
+        <v>134</v>
+      </c>
+      <c r="E868" t="s">
+        <v>7</v>
+      </c>
+      <c r="F868" t="s">
+        <v>573</v>
+      </c>
+      <c r="G868">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="869" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A869" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B869" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C869" t="s">
+        <v>1785</v>
+      </c>
+      <c r="D869" t="s">
+        <v>6</v>
+      </c>
+      <c r="E869" t="s">
+        <v>8</v>
+      </c>
+      <c r="F869" t="s">
+        <v>570</v>
+      </c>
+      <c r="G869">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="870" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A870" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B870" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C870" t="s">
+        <v>1787</v>
+      </c>
+      <c r="D870" t="s">
+        <v>113</v>
+      </c>
+      <c r="E870" t="s">
+        <v>8</v>
+      </c>
+      <c r="F870" t="s">
+        <v>570</v>
+      </c>
+      <c r="G870">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="871" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A871" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B871" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C871" t="s">
+        <v>1789</v>
+      </c>
+      <c r="D871" t="s">
+        <v>237</v>
+      </c>
+      <c r="E871" t="s">
+        <v>12</v>
+      </c>
+      <c r="F871" t="s">
+        <v>573</v>
+      </c>
+      <c r="G871">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="872" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A872" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B872" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C872" t="s">
+        <v>1791</v>
+      </c>
+      <c r="D872" t="s">
+        <v>131</v>
+      </c>
+      <c r="E872" t="s">
+        <v>7</v>
+      </c>
+      <c r="F872" t="s">
+        <v>569</v>
+      </c>
+      <c r="G872">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="873" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A873" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B873" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C873" t="s">
+        <v>1793</v>
+      </c>
+      <c r="D873" t="s">
+        <v>17</v>
+      </c>
+      <c r="E873" t="s">
+        <v>8</v>
+      </c>
+      <c r="F873" t="s">
+        <v>569</v>
+      </c>
+      <c r="G873">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="874" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A874" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B874" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C874" t="s">
+        <v>1795</v>
+      </c>
+      <c r="D874" t="s">
+        <v>131</v>
+      </c>
+      <c r="E874" t="s">
+        <v>8</v>
+      </c>
+      <c r="F874" t="s">
+        <v>570</v>
+      </c>
+      <c r="G874">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="875" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A875" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B875" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C875" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D875" t="s">
+        <v>237</v>
+      </c>
+      <c r="E875" t="s">
+        <v>12</v>
+      </c>
+      <c r="F875" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="876" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A876" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B876" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C876" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D876" t="s">
+        <v>14</v>
+      </c>
+      <c r="E876" t="s">
+        <v>8</v>
+      </c>
+      <c r="F876" t="s">
+        <v>569</v>
+      </c>
+      <c r="G876">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="877" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A877" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B877" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C877" t="s">
+        <v>1801</v>
+      </c>
+      <c r="D877" t="s">
+        <v>44</v>
+      </c>
+      <c r="E877" t="s">
+        <v>7</v>
+      </c>
+      <c r="F877" t="s">
+        <v>570</v>
+      </c>
+      <c r="G877">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="878" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A878" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B878" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C878" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D878" t="s">
+        <v>13</v>
+      </c>
+      <c r="E878" t="s">
+        <v>8</v>
+      </c>
+      <c r="F878" t="s">
+        <v>569</v>
+      </c>
+      <c r="G878">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="879" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A879" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B879" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C879" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D879" t="s">
+        <v>134</v>
+      </c>
+      <c r="E879" t="s">
+        <v>8</v>
+      </c>
+      <c r="F879" t="s">
+        <v>569</v>
+      </c>
+      <c r="G879">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="880" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A880" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B880" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C880" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D880" t="s">
+        <v>237</v>
+      </c>
+      <c r="E880" t="s">
+        <v>12</v>
+      </c>
+      <c r="F880" t="s">
+        <v>569</v>
+      </c>
+      <c r="G880">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="881" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A881" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B881" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C881" t="s">
+        <v>1809</v>
+      </c>
+      <c r="D881" t="s">
+        <v>131</v>
+      </c>
+      <c r="E881" t="s">
+        <v>8</v>
+      </c>
+      <c r="F881" t="s">
+        <v>569</v>
+      </c>
+      <c r="G881">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="882" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A882" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B882" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C882" t="s">
+        <v>1811</v>
+      </c>
+      <c r="D882" t="s">
+        <v>237</v>
+      </c>
+      <c r="E882" t="s">
+        <v>12</v>
+      </c>
+      <c r="F882" t="s">
+        <v>569</v>
+      </c>
+      <c r="G882">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="883" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A883" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B883" t="s">
+        <v>1812</v>
+      </c>
+      <c r="C883" t="s">
+        <v>1813</v>
+      </c>
+      <c r="D883" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E883" t="s">
+        <v>7</v>
+      </c>
+      <c r="F883" t="s">
+        <v>571</v>
+      </c>
+      <c r="G883" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="884" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A884" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B884" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C884" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D884" t="s">
+        <v>6</v>
+      </c>
+      <c r="E884" t="s">
+        <v>8</v>
+      </c>
+      <c r="F884" t="s">
+        <v>569</v>
+      </c>
+      <c r="G884">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="885" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A885" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B885" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C885" t="s">
+        <v>1817</v>
+      </c>
+      <c r="D885" t="s">
+        <v>154</v>
+      </c>
+      <c r="E885" t="s">
+        <v>12</v>
+      </c>
+      <c r="F885" t="s">
+        <v>573</v>
+      </c>
+      <c r="G885">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="886" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A886" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B886" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C886" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D886" t="s">
+        <v>13</v>
+      </c>
+      <c r="E886" t="s">
+        <v>8</v>
+      </c>
+      <c r="F886" t="s">
+        <v>569</v>
+      </c>
+      <c r="G886">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="887" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A887" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C887" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D887" t="s">
+        <v>1822</v>
+      </c>
+      <c r="E887" t="s">
+        <v>12</v>
+      </c>
+      <c r="F887" t="s">
+        <v>570</v>
+      </c>
+      <c r="G887">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="888" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A888" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B888" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C888" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D888" t="s">
+        <v>131</v>
+      </c>
+      <c r="E888" t="s">
+        <v>8</v>
+      </c>
+      <c r="F888" t="s">
+        <v>569</v>
+      </c>
+      <c r="G888">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="889" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A889" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B889" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C889" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D889" t="s">
+        <v>17</v>
+      </c>
+      <c r="E889" t="s">
+        <v>8</v>
+      </c>
+      <c r="F889" t="s">
+        <v>569</v>
+      </c>
+      <c r="G889">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="890" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A890" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B890" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C890" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D890" t="s">
+        <v>16</v>
+      </c>
+      <c r="E890" t="s">
+        <v>8</v>
+      </c>
+      <c r="F890" t="s">
+        <v>569</v>
+      </c>
+      <c r="G890">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="891" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A891" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B891" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C891" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D891" t="s">
+        <v>22</v>
+      </c>
+      <c r="E891" t="s">
+        <v>8</v>
+      </c>
+      <c r="F891" t="s">
+        <v>569</v>
+      </c>
+      <c r="G891">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="892" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A892" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B892" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C892" t="s">
+        <v>1832</v>
+      </c>
+      <c r="D892" t="s">
+        <v>134</v>
+      </c>
+      <c r="E892" t="s">
+        <v>8</v>
+      </c>
+      <c r="F892" t="s">
+        <v>570</v>
+      </c>
+      <c r="G892">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="893" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A893" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B893" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C893" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D893" t="s">
+        <v>116</v>
+      </c>
+      <c r="E893" t="s">
+        <v>8</v>
+      </c>
+      <c r="F893" t="s">
+        <v>569</v>
+      </c>
+      <c r="G893">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="894" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A894" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B894" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C894" t="s">
+        <v>1836</v>
+      </c>
+      <c r="D894" t="s">
+        <v>13</v>
+      </c>
+      <c r="E894" t="s">
+        <v>8</v>
+      </c>
+      <c r="F894" t="s">
+        <v>569</v>
+      </c>
+      <c r="G894">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="895" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A895" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B895" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C895" t="s">
+        <v>1838</v>
+      </c>
+      <c r="D895" t="s">
+        <v>10</v>
+      </c>
+      <c r="E895" t="s">
+        <v>8</v>
+      </c>
+      <c r="F895" t="s">
+        <v>573</v>
+      </c>
+      <c r="G895">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="896" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A896" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B896" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C896" t="s">
+        <v>1840</v>
+      </c>
+      <c r="D896" t="s">
+        <v>14</v>
+      </c>
+      <c r="E896" t="s">
+        <v>8</v>
+      </c>
+      <c r="F896" t="s">
+        <v>568</v>
+      </c>
+      <c r="G896">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="897" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A897" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B897" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C897" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D897" t="s">
+        <v>22</v>
+      </c>
+      <c r="E897" t="s">
+        <v>7</v>
+      </c>
+      <c r="F897" t="s">
+        <v>570</v>
+      </c>
+      <c r="G897">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="898" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A898" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B898" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C898" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D898" t="s">
+        <v>113</v>
+      </c>
+      <c r="E898" t="s">
+        <v>8</v>
+      </c>
+      <c r="F898" t="s">
+        <v>569</v>
+      </c>
+      <c r="G898">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="899" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A899" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B899" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C899" t="s">
+        <v>1846</v>
+      </c>
+      <c r="D899" t="s">
+        <v>134</v>
+      </c>
+      <c r="E899" t="s">
+        <v>8</v>
+      </c>
+      <c r="F899" t="s">
+        <v>569</v>
+      </c>
+      <c r="G899">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="900" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A900" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B900" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C900" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D900" t="s">
+        <v>131</v>
+      </c>
+      <c r="E900" t="s">
+        <v>8</v>
+      </c>
+      <c r="F900" t="s">
+        <v>569</v>
+      </c>
+      <c r="G900">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="901" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A901" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B901" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C901" t="s">
+        <v>1850</v>
+      </c>
+      <c r="D901" t="s">
+        <v>237</v>
+      </c>
+      <c r="E901" t="s">
+        <v>12</v>
+      </c>
+      <c r="F901" t="s">
+        <v>569</v>
+      </c>
+      <c r="G901">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="902" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A902" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B902" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C902" t="s">
+        <v>1852</v>
+      </c>
+      <c r="D902" t="s">
+        <v>134</v>
+      </c>
+      <c r="E902" t="s">
+        <v>8</v>
+      </c>
+      <c r="F902" t="s">
+        <v>569</v>
+      </c>
+      <c r="G902">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="903" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A903" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B903" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C903" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D903" t="s">
+        <v>22</v>
+      </c>
+      <c r="E903" t="s">
+        <v>7</v>
+      </c>
+      <c r="F903" t="s">
+        <v>570</v>
+      </c>
+      <c r="G903">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="904" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A904" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B904" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C904" t="s">
+        <v>1856</v>
+      </c>
+      <c r="D904" t="s">
+        <v>237</v>
+      </c>
+      <c r="E904" t="s">
+        <v>12</v>
+      </c>
+      <c r="F904" t="s">
+        <v>568</v>
+      </c>
+      <c r="G904">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="905" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A905" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B905" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C905" t="s">
+        <v>1858</v>
+      </c>
+      <c r="D905" t="s">
+        <v>16</v>
+      </c>
+      <c r="E905" t="s">
+        <v>8</v>
+      </c>
+      <c r="F905" t="s">
+        <v>569</v>
+      </c>
+      <c r="G905">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="906" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A906" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B906" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C906" t="s">
+        <v>1860</v>
+      </c>
+      <c r="D906" t="s">
+        <v>116</v>
+      </c>
+      <c r="E906" t="s">
+        <v>8</v>
+      </c>
+      <c r="F906" t="s">
+        <v>570</v>
+      </c>
+      <c r="G906">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="907" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A907" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B907" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C907" t="s">
+        <v>1862</v>
+      </c>
+      <c r="D907" t="s">
+        <v>1822</v>
+      </c>
+      <c r="E907" t="s">
+        <v>12</v>
+      </c>
+      <c r="F907" t="s">
+        <v>569</v>
+      </c>
+      <c r="G907">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="908" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A908" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B908" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C908" t="s">
+        <v>1864</v>
+      </c>
+      <c r="D908" t="s">
+        <v>1822</v>
+      </c>
+      <c r="E908" t="s">
+        <v>12</v>
+      </c>
+      <c r="F908" t="s">
+        <v>569</v>
+      </c>
+      <c r="G908">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="909" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A909" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B909" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C909" t="s">
+        <v>1866</v>
+      </c>
+      <c r="D909" t="s">
+        <v>134</v>
+      </c>
+      <c r="E909" t="s">
+        <v>8</v>
+      </c>
+      <c r="F909" t="s">
+        <v>569</v>
+      </c>
+      <c r="G909">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="910" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A910" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B910" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C910" t="s">
+        <v>1868</v>
+      </c>
+      <c r="D910" t="s">
+        <v>237</v>
+      </c>
+      <c r="E910" t="s">
+        <v>12</v>
+      </c>
+      <c r="F910" t="s">
+        <v>569</v>
+      </c>
+      <c r="G910">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="911" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A911" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B911" t="s">
+        <v>1869</v>
+      </c>
+      <c r="C911" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D911" t="s">
+        <v>116</v>
+      </c>
+      <c r="E911" t="s">
+        <v>8</v>
+      </c>
+      <c r="F911" t="s">
+        <v>569</v>
+      </c>
+      <c r="G911">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="912" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A912" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B912" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C912" t="s">
+        <v>1872</v>
+      </c>
+      <c r="D912" t="s">
+        <v>116</v>
+      </c>
+      <c r="E912" t="s">
+        <v>8</v>
+      </c>
+      <c r="F912" t="s">
+        <v>569</v>
+      </c>
+      <c r="G912">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="913" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A913" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B913" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C913" t="s">
+        <v>1874</v>
+      </c>
+      <c r="D913" t="s">
+        <v>13</v>
+      </c>
+      <c r="E913" t="s">
+        <v>8</v>
+      </c>
+      <c r="F913" t="s">
+        <v>569</v>
+      </c>
+      <c r="G913">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="914" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A914" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B914" t="s">
+        <v>1875</v>
+      </c>
+      <c r="C914" t="s">
+        <v>1876</v>
+      </c>
+      <c r="D914" t="s">
+        <v>13</v>
+      </c>
+      <c r="E914" t="s">
+        <v>8</v>
+      </c>
+      <c r="F914" t="s">
+        <v>569</v>
+      </c>
+      <c r="G914">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="915" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A915" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B915" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C915" t="s">
+        <v>1878</v>
+      </c>
+      <c r="D915" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E915" t="s">
+        <v>7</v>
+      </c>
+      <c r="F915" t="s">
+        <v>568</v>
+      </c>
+      <c r="G915">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="916" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A916" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B916" t="s">
+        <v>1879</v>
+      </c>
+      <c r="C916" t="s">
+        <v>1880</v>
+      </c>
+      <c r="D916" t="s">
+        <v>22</v>
+      </c>
+      <c r="E916" t="s">
+        <v>7</v>
+      </c>
+      <c r="F916" t="s">
+        <v>568</v>
+      </c>
+      <c r="G916">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="917" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A917" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B917" t="s">
+        <v>1881</v>
+      </c>
+      <c r="C917" t="s">
+        <v>1882</v>
+      </c>
+      <c r="D917" t="s">
+        <v>16</v>
+      </c>
+      <c r="E917" t="s">
+        <v>8</v>
+      </c>
+      <c r="F917" t="s">
+        <v>569</v>
+      </c>
+      <c r="G917">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="918" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A918" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B918" t="s">
+        <v>1883</v>
+      </c>
+      <c r="C918" t="s">
+        <v>1884</v>
+      </c>
+      <c r="D918" t="s">
+        <v>17</v>
+      </c>
+      <c r="E918" t="s">
+        <v>8</v>
+      </c>
+      <c r="F918" t="s">
+        <v>569</v>
+      </c>
+      <c r="G918">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="919" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A919" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B919" t="s">
+        <v>1885</v>
+      </c>
+      <c r="C919" t="s">
+        <v>1886</v>
+      </c>
+      <c r="D919" t="s">
+        <v>14</v>
+      </c>
+      <c r="E919" t="s">
+        <v>8</v>
+      </c>
+      <c r="F919" t="s">
+        <v>569</v>
+      </c>
+      <c r="G919">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="920" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A920" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B920" t="s">
+        <v>1887</v>
+      </c>
+      <c r="C920" t="s">
+        <v>1888</v>
+      </c>
+      <c r="D920" t="s">
+        <v>1822</v>
+      </c>
+      <c r="E920" t="s">
+        <v>12</v>
+      </c>
+      <c r="F920" t="s">
+        <v>569</v>
+      </c>
+      <c r="G920">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="921" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A921" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B921" t="s">
+        <v>1889</v>
+      </c>
+      <c r="C921" t="s">
+        <v>1890</v>
+      </c>
+      <c r="D921" t="s">
+        <v>1891</v>
+      </c>
+      <c r="E921" t="s">
+        <v>12</v>
+      </c>
+      <c r="F921" t="s">
+        <v>569</v>
+      </c>
+      <c r="G921">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="922" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A922" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B922" t="s">
+        <v>1892</v>
+      </c>
+      <c r="C922" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D922" t="s">
+        <v>134</v>
+      </c>
+      <c r="E922" t="s">
+        <v>8</v>
+      </c>
+      <c r="F922" t="s">
+        <v>569</v>
+      </c>
+      <c r="G922">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="923" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A923" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B923" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C923" t="s">
+        <v>1895</v>
+      </c>
+      <c r="D923" t="s">
+        <v>13</v>
+      </c>
+      <c r="E923" t="s">
+        <v>8</v>
+      </c>
+      <c r="F923" t="s">
+        <v>573</v>
+      </c>
+      <c r="G923">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="924" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A924" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B924" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C924" t="s">
+        <v>1897</v>
+      </c>
+      <c r="D924" t="s">
+        <v>1822</v>
+      </c>
+      <c r="E924" t="s">
+        <v>12</v>
+      </c>
+      <c r="F924" t="s">
+        <v>569</v>
+      </c>
+      <c r="G924">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="925" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A925" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B925" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C925" t="s">
+        <v>1899</v>
+      </c>
+      <c r="D925" t="s">
+        <v>16</v>
+      </c>
+      <c r="E925" t="s">
+        <v>8</v>
+      </c>
+      <c r="F925" t="s">
+        <v>568</v>
+      </c>
+      <c r="G925">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="926" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A926" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B926" t="s">
+        <v>1900</v>
+      </c>
+      <c r="C926" t="s">
+        <v>1901</v>
+      </c>
+      <c r="D926" t="s">
+        <v>6</v>
+      </c>
+      <c r="E926" t="s">
+        <v>8</v>
+      </c>
+      <c r="F926" t="s">
+        <v>569</v>
+      </c>
+      <c r="G926">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="927" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A927" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B927" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C927" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D927" t="s">
+        <v>9</v>
+      </c>
+      <c r="E927" t="s">
+        <v>8</v>
+      </c>
+      <c r="F927" t="s">
+        <v>569</v>
+      </c>
+      <c r="G927">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="928" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A928" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B928" t="s">
+        <v>1904</v>
+      </c>
+      <c r="C928" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D928" t="s">
+        <v>11</v>
+      </c>
+      <c r="E928" t="s">
+        <v>8</v>
+      </c>
+      <c r="F928" t="s">
+        <v>573</v>
+      </c>
+      <c r="G928">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="929" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A929" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B929" t="s">
+        <v>1906</v>
+      </c>
+      <c r="C929" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D929" t="s">
+        <v>22</v>
+      </c>
+      <c r="E929" t="s">
+        <v>8</v>
+      </c>
+      <c r="F929" t="s">
+        <v>569</v>
+      </c>
+      <c r="G929">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="930" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A930" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B930" t="s">
+        <v>1908</v>
+      </c>
+      <c r="C930" t="s">
+        <v>1909</v>
+      </c>
+      <c r="D930" t="s">
+        <v>44</v>
+      </c>
+      <c r="E930" t="s">
+        <v>7</v>
+      </c>
+      <c r="F930" t="s">
+        <v>573</v>
+      </c>
+      <c r="G930">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="931" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A931" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B931" t="s">
+        <v>1910</v>
+      </c>
+      <c r="C931" t="s">
+        <v>1911</v>
+      </c>
+      <c r="D931" t="s">
+        <v>9</v>
+      </c>
+      <c r="E931" t="s">
+        <v>8</v>
+      </c>
+      <c r="F931" t="s">
+        <v>569</v>
+      </c>
+      <c r="G931">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="932" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A932" s="1">
+        <v>46038</v>
+      </c>
+      <c r="B932" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C932" t="s">
+        <v>1913</v>
+      </c>
+      <c r="D932" t="s">
+        <v>116</v>
+      </c>
+      <c r="E932" t="s">
+        <v>8</v>
+      </c>
+      <c r="F932" t="s">
+        <v>573</v>
+      </c>
+      <c r="G932">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="933" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A933" s="1">
+        <v>46041</v>
+      </c>
+      <c r="B933" t="s">
+        <v>1914</v>
+      </c>
+      <c r="C933" t="s">
+        <v>1915</v>
+      </c>
+      <c r="D933" t="s">
+        <v>16</v>
+      </c>
+      <c r="E933" t="s">
+        <v>8</v>
+      </c>
+      <c r="F933" t="s">
+        <v>569</v>
+      </c>
+      <c r="G933">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="934" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A934" s="1">
+        <v>46041</v>
+      </c>
+      <c r="B934" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C934" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D934" t="s">
+        <v>6</v>
+      </c>
+      <c r="E934" t="s">
+        <v>8</v>
+      </c>
+      <c r="F934" t="s">
+        <v>569</v>
+      </c>
+      <c r="G934">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="935" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A935" s="1">
+        <v>46041</v>
+      </c>
+      <c r="B935" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C935" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D935" t="s">
+        <v>134</v>
+      </c>
+      <c r="E935" t="s">
+        <v>8</v>
+      </c>
+      <c r="F935" t="s">
+        <v>569</v>
+      </c>
+      <c r="G935">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="936" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A936" s="1">
+        <v>46041</v>
+      </c>
+      <c r="B936" t="s">
+        <v>1920</v>
+      </c>
+      <c r="C936" t="s">
+        <v>1921</v>
+      </c>
+      <c r="D936" t="s">
+        <v>23</v>
+      </c>
+      <c r="E936" t="s">
+        <v>8</v>
+      </c>
+      <c r="F936" t="s">
+        <v>569</v>
+      </c>
+      <c r="G936">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="937" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A937" s="1">
+        <v>46041</v>
+      </c>
+      <c r="B937" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C937" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D937" t="s">
+        <v>134</v>
+      </c>
+      <c r="E937" t="s">
+        <v>8</v>
+      </c>
+      <c r="F937" t="s">
+        <v>569</v>
+      </c>
+      <c r="G937">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="938" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A938" s="1"/>
     </row>
-    <row r="939" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A939" s="1"/>
     </row>
-    <row r="940" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A940" s="1"/>
     </row>
-    <row r="941" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A941" s="1"/>
     </row>
-    <row r="942" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A942" s="1"/>
     </row>
-    <row r="943" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A943" s="1"/>
     </row>
-    <row r="944" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A944" s="1"/>
     </row>
     <row r="945" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated balde and producao - base 23/01/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-01.xlsx
+++ b/first-atlas/producao_2026-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A10EA5-885A-4359-B8D6-B005C8996ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C789715F-45E2-4FE8-AC52-25192D9F4095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
@@ -8360,7 +8360,7 @@
   <dimension ref="A1:G1297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>